<commit_message>
Ran validation scripts and with jaccard similarity
</commit_message>
<xml_diff>
--- a/validation/final_paper_selection.xlsx
+++ b/validation/final_paper_selection.xlsx
@@ -566,7 +566,7 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>("software maintenance" OR "software evolution" OR "legacy systems") AND ("globally distributed" OR "distributed teams" OR "offshore development" OR "global software engineering") AND ("challenges" OR "problems" OR "issues" OR "difficulties" OR "obstacles") AND ("mitigation" OR "resolution" OR "strategies" OR "approaches" OR "solutions" OR "best practices")</t>
+          <t>("software maintenance" OR "software evolution" OR "legacy systems" OR "technical debt") AND ("globally distributed settings" OR "distributed software development" OR "offshore development" OR "global software engineering") AND ("challenges" OR "difficulties" OR "problems" OR "issues" OR "obstacles") AND ("mitigation strategies" OR "coping mechanisms" OR "solutions" OR "best practices" OR "management strategies")</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -576,11 +576,11 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>['approaches', 'best practices', 'challenges', 'difficulties', 'distributed teams', 'global software engineering', 'globally distributed', 'issues', 'legacy systems', 'mitigation', 'obstacles', 'offshore development', 'problems', 'resolution', 'software evolution', 'software maintenance', 'solutions', 'strategies']</t>
+          <t>['best practices', 'challenges', 'coping mechanisms', 'difficulties', 'distributed software development', 'global software engineering', 'globally distributed settings', 'issues', 'legacy systems', 'management strategies', 'mitigation strategies', 'obstacles', 'offshore development', 'problems', 'software evolution', 'software maintenance', 'solutions', 'technical debt']</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.03125</v>
+        <v>0.06451612903225806</v>
       </c>
     </row>
     <row r="3">
@@ -635,7 +635,7 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>("success factors" OR "critical success factors" OR "enablers" OR "drivers") AND ("chief data officer" OR "CDO" OR "data leader" OR "data governance") AND ("literature review" OR "expert opinion" OR "questionnaire" OR "survey") AND ("prioritization" OR "taxonomy" OR "classification" OR "framework")</t>
+          <t>("Cloud Software Development Optimization" OR "Cloud Software Development" OR "Software Development Optimization" OR CSDO) AND ("success factors" OR "critical success factors" OR "key success factors" OR enablers OR drivers OR determinants) AND (findings OR research OR studies OR literature) AND ("expert perspectives" OR "expert views" OR "industry experts" OR practitioners) AND (prioritization OR ranking OR taxonomy OR classification OR categorization)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -645,11 +645,11 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>['cdo', 'chief data officer', 'classification', 'critical success factors', 'data governance', 'data leader', 'drivers', 'enablers', 'expert opinion', 'framework', 'literature review', 'prioritization', 'questionnaire', 'success factors', 'survey', 'taxonomy']</t>
+          <t>['categorization', 'classification', 'cloud software development', 'cloud software development optimization', 'critical success factors', 'csdo', 'determinants', 'drivers', 'enablers', 'expert perspectives', 'expert views', 'findings', 'industry experts', 'key success factors', 'literature', 'practitioners', 'prioritization', 'ranking', 'research', 'software development optimization', 'studies', 'success factors', 'taxonomy']</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0.05</v>
+        <v>0.0425531914893617</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>("model transformation" OR "model transformations") AND ("design pattern" OR "design patterns" OR "pattern language") AND ("MT development" OR "model transformation development") AND (practice OR application OR usage) AND (categories OR types OR classification) AND (explicit OR recognized) AND (benefits OR advantages OR outcomes) AND (adoption OR trend OR evolution) AND (languages OR frameworks OR tools)</t>
+          <t>("model transformation" OR "metamodeling" OR "transformation languages") AND ("design patterns" OR "pattern application") AND (practice OR "empirical studies" OR "industrial experience") AND (categories OR types) AND (explicit OR implicit) AND (benefits OR advantages) AND ("adoption over time" OR trends)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -708,11 +708,11 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>['adoption', 'advantages', 'application', 'benefits', 'categories', 'classification', 'design pattern', 'design patterns', 'evolution', 'explicit', 'frameworks', 'languages', 'model transformation', 'model transformation development', 'model transformations', 'mt development', 'outcomes', 'pattern language', 'practice', 'recognized', 'tools', 'trend', 'types', 'usage']</t>
+          <t>['adoption over time', 'advantages', 'benefits', 'categories', 'design patterns', 'empirical studies', 'explicit', 'implicit', 'industrial experience', 'metamodeling', 'model transformation', 'pattern application', 'practice', 'transformation languages', 'trends', 'types']</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="5">
@@ -764,7 +764,7 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>("blockchain governance" OR "decentralized governance" OR "on-chain governance" OR "distributed governance") AND ("building blocks" OR "components" OR "elements" OR "framework" OR "architecture")</t>
+          <t>("blockchain governance" OR "distributed ledger governance" OR blockchain) AND ("building blocks" OR components OR elements OR framework OR infrastructure OR foundations OR architecture)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>['architecture', 'blockchain governance', 'building blocks', 'components', 'decentralized governance', 'distributed governance', 'elements', 'framework', 'on-chain governance']</t>
+          <t>['architecture', 'blockchain', 'blockchain governance', 'building blocks', 'components', 'distributed ledger governance', 'elements', 'foundations', 'framework', 'infrastructure']</t>
         </is>
       </c>
       <c r="Q5" t="n">
@@ -827,7 +827,7 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>("mortality compression" OR "MCR") AND ("approaches" OR "methods" OR "strategies") AND ("evaluation" OR "assessment" OR "outcomes") AND ("conclusions" OR "findings" OR "results")</t>
+          <t>("Model Car Racing" OR MCR OR "miniature car racing" OR "radio-controlled car racing") AND ("theory" OR "principles" OR "framework" OR "knowledge base") AND ("method" OR "technique" OR "strategy" OR "support") AND ("evaluation" OR "assessment" OR "validation" OR "conclusion" OR "result" OR "outcome")</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>['approaches', 'assessment', 'conclusions', 'evaluation', 'findings', 'mcr', 'methods', 'mortality compression', 'outcomes', 'results', 'strategies']</t>
+          <t>['assessment', 'conclusion', 'evaluation', 'framework', 'knowledge base', 'mcr', 'method', 'miniature car racing', 'model car racing', 'outcome', 'principles', 'radio-controlled car racing', 'result', 'strategy', 'support', 'technique', 'theory', 'validation']</t>
         </is>
       </c>
       <c r="Q6" t="n">
@@ -888,7 +888,11 @@
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>("visual notation" OR "visual notations" OR diagram OR diagrams OR model OR models OR "graphical representation" OR "graphical representations") AND ("Physics of Notations" OR "PoN theory" OR "PoN") AND (analysis OR analyzed OR "analyzing") AND ("user requirements" OR "notation user" OR "user experience") AND (verifiable OR verification OR "analysis validity")</t>
+        </is>
+      </c>
       <c r="O7" t="inlineStr">
         <is>
           <t>['“cognitive effectiveness”', '“diagram”', '“language”', '“modeling”', '“notation”', '“physics of notations”', '“visual”']</t>
@@ -896,7 +900,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>['nan']</t>
+          <t>['analysis', 'analysis validity', 'analyzed', 'analyzing', 'diagram', 'diagrams', 'graphical representation', 'graphical representations', 'model', 'models', 'notation user', 'physics of notations', 'pon', 'pon theory', 'user experience', 'user requirements', 'verifiable', 'verification', 'visual notation', 'visual notations']</t>
         </is>
       </c>
       <c r="Q7" t="n">
@@ -949,7 +953,7 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>(("semi-automatic configuration" OR "automated configuration" OR "assisted configuration") AND ("product line" OR "product family" OR "software product line") AND ("techniques" OR "methods" OR "approaches") AND ("evaluation" OR "validation" OR "assessment") AND ("challenges" OR "limitations" OR "open issues"))</t>
+          <t>("semi-automatic configuration" OR "assisted configuration" OR "partially automated configuration" OR "configuration") AND ("extended product lines" OR "software product lines" OR "SPL" OR "product family") AND (evaluation OR validation OR experiment OR "case study" OR "performance analysis") AND ("open challenges" OR limitations OR "future research" OR "unresolved issues")</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -959,11 +963,11 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>['approaches', 'assessment', 'assisted configuration', 'automated configuration', 'challenges', 'evaluation', 'limitations', 'methods', 'open issues', 'product family', 'product line', 'semi-automatic configuration', 'software product line', 'techniques', 'validation']</t>
+          <t>['assisted configuration', 'case study', 'configuration', 'evaluation', 'experiment', 'extended product lines', 'future research', 'limitations', 'open challenges', 'partially automated configuration', 'performance analysis', 'product family', 'semi-automatic configuration', 'software product lines', 'spl', 'unresolved issues', 'validation']</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.03703703703703703</v>
       </c>
     </row>
     <row r="9">
@@ -1049,7 +1053,7 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>("Deep Learning" OR "Deep Neural Networks" OR "Machine Learning") AND ("Software Engineering" OR "Software Development" OR "Software Maintenance") AND (Tasks OR Applications) AND (Data Extraction OR Data Preprocessing) AND (Model Architecture OR Learning Algorithms) AND (Performance Evaluation OR Benchmarks) AND (Reproducibility OR Replication)</t>
+          <t>("deep learning" OR "neural networks" OR "machine learning") AND ("software engineering" OR "software development" OR "software design" OR "software maintenance") AND (data OR artifacts) AND (extraction OR preprocessing) AND (model OR architecture OR training) AND (evaluation OR benchmark) AND (reproducibility OR replication)</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1059,7 +1063,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>['applications', 'benchmarks', 'data extraction', 'data preprocessing', 'deep learning', 'deep neural networks', 'learning algorithms', 'machine learning', 'model architecture', 'performance evaluation', 'replication', 'reproducibility', 'software development', 'software engineering', 'software maintenance', 'tasks']</t>
+          <t>['architecture', 'artifacts', 'benchmark', 'data', 'deep learning', 'evaluation', 'extraction', 'machine learning', 'model', 'neural networks', 'preprocessing', 'replication', 'reproducibility', 'software design', 'software development', 'software engineering', 'software maintenance', 'training']</t>
         </is>
       </c>
       <c r="Q9" t="n">
@@ -1116,7 +1120,7 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>("software trust" OR "SECO trust" OR "security trust") AND (definition OR concept OR meaning) AND (("software product" OR "software version" OR "software package manager" OR "software organization" OR "software engineer") AND (selection OR choosing OR decision-making) AND (trust OR trustworthiness OR reliability OR security OR safety OR integrity OR reputation OR assurance))</t>
+          <t>("software trust" OR "trustworthiness of software" OR "confidence in software") AND (definition OR concept OR understanding) OR ("SECO trust" OR "secure coding trust") AND (definition OR concept OR understanding) OR ("software product selection" OR "software version selection") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users") OR ("software package managers") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users") OR ("software producing organizations") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users") OR ("software engineers") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users")</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1126,11 +1130,11 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>['assurance', 'choosing', 'concept', 'decision-making', 'definition', 'integrity', 'meaning', 'reliability', 'reputation', 'safety', 'seco trust', 'security', 'security trust', 'selection', 'software engineer', 'software organization', 'software package manager', 'software product', 'software trust', 'software version', 'trust', 'trustworthiness']</t>
+          <t>['concept', 'concept', 'confidence in software', 'definition', 'definition', 'end-user organizations', 'end-user organizations', 'end-user organizations', 'end-user organizations', 'seco trust', 'secure coding trust', 'software engineers', 'software package managers', 'software producing organizations', 'software product selection', 'software trust', 'software version selection', 'trust evaluation criteria', 'trust evaluation criteria', 'trust evaluation criteria', 'trust evaluation criteria', 'trust factors', 'trust factors', 'trust factors', 'trust factors', 'trust indicators', 'trust indicators', 'trust indicators', 'trust indicators', 'trust metrics', 'trust metrics', 'trust metrics', 'trust metrics', 'trustworthiness of software', 'understanding', 'understanding', 'users', 'users', 'users', 'users']</t>
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>0.0625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1179,7 +1183,7 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>("data mining" OR "machine learning" OR "text mining" OR "sentiment analysis" OR "topic modeling" OR "classification" OR "clustering" OR "regression") AND ("app store" OR "Google Play" OR "Apple App Store") AND ("software review" OR "app review") AND ("domain adaptation" OR "transfer learning" OR "cross-domain" OR "domain shift" OR "contextual variation") AND ("review helpfulness" OR "review quality" OR "review credibility" OR "review informativeness" OR "accuracy" OR "relevance" OR "completeness" OR "timeliness" OR "specificity") AND ("spam detection" OR "fraudulent review" OR "fake review" OR "deceptive review") AND ("feature extraction" OR "aspect extraction" OR "information extraction" OR "entity recognition") AND ("software feature" OR "app feature" OR "performance" OR "usability" OR "security" OR "functionality")</t>
+          <t>("data mining" OR "data analysis" OR "machine learning") AND ("software distribution platform" OR "app store" OR "application store") AND (review OR reviews) AND (usefulness OR helpfulness OR quality) AND ("spam review" OR "fake review" OR "deceptive review") AND (legitimate OR genuine OR authentic) AND ("software feature" OR "application feature" OR "functionality") AND (extraction OR mining OR identification) AND ("domain dependency" OR "context dependency")</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1189,11 +1193,11 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>['accuracy', 'app feature', 'app review', 'app store', 'apple app store', 'aspect extraction', 'classification', 'clustering', 'completeness', 'contextual variation', 'cross-domain', 'data mining', 'deceptive review', 'domain adaptation', 'domain shift', 'entity recognition', 'fake review', 'feature extraction', 'fraudulent review', 'functionality', 'google play', 'information extraction', 'machine learning', 'performance', 'regression', 'relevance', 'review credibility', 'review helpfulness', 'review informativeness', 'review quality', 'security', 'sentiment analysis', 'software feature', 'software review', 'spam detection', 'specificity', 'text mining', 'timeliness', 'topic modeling', 'transfer learning', 'usability']</t>
+          <t>['app store', 'application feature', 'application store', 'authentic', 'context dependency', 'data analysis', 'data mining', 'deceptive review', 'domain dependency', 'extraction', 'fake review', 'functionality', 'genuine', 'helpfulness', 'identification', 'legitimate', 'machine learning', 'mining', 'quality', 'review', 'reviews', 'software distribution platform', 'software feature', 'spam review', 'usefulness']</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>0.09615384615384616</v>
       </c>
     </row>
     <row r="12">
@@ -1242,7 +1246,11 @@
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>("visualization techniques" OR "visual representation" OR "data visualization") AND ("software architecture" OR "architectural design" OR "system architecture" OR "software design") AND ("architecting process" OR "architecting activities" OR "architecture visualization tools" OR "software visualization")</t>
+        </is>
+      </c>
       <c r="O12" t="inlineStr">
         <is>
           <t>['architecting', 'architectural', 'architecture', 'diagram', 'graphic', 'graphical', 'picture', 'structure', 'visual', 'visualization', 'visualize', 'visualizing']</t>
@@ -1250,7 +1258,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>['nan']</t>
+          <t>['architecting activities', 'architecting process', 'architectural design', 'architecture visualization tools', 'data visualization', 'software architecture', 'software design', 'software visualization', 'system architecture', 'visual representation', 'visualization techniques']</t>
         </is>
       </c>
       <c r="Q12" t="n">
@@ -1309,7 +1317,7 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
-          <t>("UML" OR "Unified Modeling Language") AND ("consistency" OR "validation" OR "verification") AND ("diagram" OR "model") AND ("formal method" OR "formal technique" OR "non-formal method" OR "non-formal technique") AND ("version" OR "revision") AND ("check" OR "rule" OR "constraint")</t>
+          <t>("Unified Modeling Language" OR UML) AND (consistency OR integrity OR validation) AND ("formal method" OR "non-formal method" OR technique OR language) AND (diagram OR "class diagram" OR "sequence diagram" OR "activity diagram" OR "state diagram" OR "use case diagram") AND ("consistency check*" OR "integrity check*" OR "validation check*" OR "error detection") AND (extend* OR support OR new)</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -1319,7 +1327,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>['check', 'consistency', 'constraint', 'diagram', 'formal method', 'formal technique', 'model', 'non-formal method', 'non-formal technique', 'revision', 'rule', 'uml', 'unified modeling language', 'validation', 'verification', 'version']</t>
+          <t>['activity diagram', 'class diagram', 'consistency', 'consistency check*', 'diagram', 'error detection', 'extend*', 'formal method', 'integrity', 'integrity check*', 'language', 'new', 'non-formal method', 'sequence diagram', 'state diagram', 'support', 'technique', 'uml', 'unified modeling language', 'use case diagram', 'validation', 'validation check*']</t>
         </is>
       </c>
       <c r="Q13" t="n">
@@ -1385,7 +1393,7 @@
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
-          <t>("Search Based Software Testing" OR SBST) AND ("Mutation Testing" OR "Fault Injection") AND (Meta-heuristics OR "Genetic Algorithm" OR "Simulated Annealing" OR "Evolutionary Algorithm") AND ("Fitness Functions") AND ("Programming Languages")</t>
+          <t>("Search Based Software Testing" OR "search-based software testing" OR "search based software testing" OR "optimization-based software testing" OR "search algorithms for software testing") AND ("mutation testing" OR "mutation analysis" OR "mutation operators" OR "mutants") AND ("genetic algorithms" OR "simulated annealing" OR "particle swarm optimization" OR "evolutionary algorithms") AND ("fitness functions" OR "objective functions" OR "evaluation functions") AND ("mutation generation" OR "mutation execution" OR "mutation analysis") AND ("programming languages")</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
@@ -1395,11 +1403,11 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>['evolutionary algorithm', 'fault injection', 'fitness functions', 'genetic algorithm', 'meta-heuristics', 'mutation testing', 'programming languages', 'sbst', 'search based software testing', 'simulated annealing']</t>
+          <t>['evaluation functions', 'evolutionary algorithms', 'fitness functions', 'genetic algorithms', 'mutants', 'mutation analysis', 'mutation analysis', 'mutation execution', 'mutation generation', 'mutation operators', 'mutation testing', 'objective functions', 'optimization-based software testing', 'particle swarm optimization', 'programming languages', 'search algorithms for software testing', 'search based software testing', 'search based software testing', 'search-based software testing', 'simulated annealing']</t>
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>0.07407407407407407</v>
+        <v>0.1212121212121212</v>
       </c>
     </row>
     <row r="15">
@@ -1453,7 +1461,11 @@
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>("code smell" OR "code smells" OR "software smell" OR "software smells" OR "bad code smell" OR "poor code quality") AND ("experiment" OR "empirical study") AND ("theme" OR "finding" OR "result") AND ("comparison" OR "convergence")</t>
+        </is>
+      </c>
       <c r="O15" t="inlineStr">
         <is>
           <t>['anti-patternandexperiment', 'controlled', 'disharmony', 'empirical', 'ethnography', 'smell', 'study', 'survey', '“action research”', '“code anomaly”', '“design anomaly”', '“design flaw”', '“exploratory analysis”']</t>
@@ -1461,7 +1473,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>['nan']</t>
+          <t>['bad code smell', 'code smell', 'code smells', 'comparison', 'convergence', 'empirical study', 'experiment', 'finding', 'poor code quality', 'result', 'software smell', 'software smells', 'theme']</t>
         </is>
       </c>
       <c r="Q15" t="n">
@@ -1515,7 +1527,7 @@
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
-          <t>("Strategic Information Systems" OR "Strategic IS" OR SIA) AND (Inputs OR Data OR Resources OR "Input Factors") AND (Processes OR Methods OR Workflows OR Procedures) AND (Outputs OR Results OR Outcomes OR Deliverables) AND (Usability OR Effectiveness OR "User Experience" OR Adoption)</t>
+          <t>("socially intelligent agent*" OR "social agent*" OR "intelligent agent*" OR SIA) AND (input* OR "data source*" OR "information source*" OR feed*) AND (process* OR method* OR technique* OR algorithm*) AND (output* OR result* OR outcome* OR product*) AND (usability OR "ease of use" OR "user experience" OR UX OR accessibility OR acceptance)</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1525,7 +1537,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>['adoption', 'data', 'deliverables', 'effectiveness', 'input factors', 'inputs', 'methods', 'outcomes', 'outputs', 'procedures', 'processes', 'resources', 'results', 'sia', 'strategic information systems', 'strategic is', 'usability', 'user experience', 'workflows']</t>
+          <t>['acceptance', 'accessibility', 'algorithm*', 'data source*', 'ease of use', 'feed*', 'information source*', 'input*', 'intelligent agent*', 'method*', 'outcome*', 'output*', 'process*', 'product*', 'result*', 'sia', 'social agent*', 'socially intelligent agent*', 'technique*', 'usability', 'user experience', 'ux']</t>
         </is>
       </c>
       <c r="Q16" t="n">
@@ -1599,7 +1611,7 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr">
         <is>
-          <t>("agile method" OR "agile methods" OR "Scrum" OR "XP" OR "Extreme Programming" OR "Kanban") AND ("method tailoring" OR "method adaptation" OR "method customization" OR "method configuration") AND ("research methods" OR "study design" OR "data collection" OR "case studies" OR "implementation" OR "evaluation" OR "context factors" OR "project characteristics" OR "organizational needs")</t>
+          <t>("agile method" OR "agile methods" OR "scrum" OR "kanban" OR "lean") AND ("method tailoring" OR "method adaptation" OR "method customization" OR "method configuration") AND ("methodology" OR "approach" OR "framework" OR "process") AND ("practical" OR "empirical" OR "evaluation" OR "application") AND ("criteria" OR "factors" OR "metrics" OR "guidelines")</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -1609,7 +1621,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>['agile method', 'agile methods', 'case studies', 'context factors', 'data collection', 'evaluation', 'extreme programming', 'implementation', 'kanban', 'method adaptation', 'method configuration', 'method customization', 'method tailoring', 'organizational needs', 'project characteristics', 'research methods', 'scrum', 'study design', 'xp']</t>
+          <t>['agile method', 'agile methods', 'application', 'approach', 'criteria', 'empirical', 'evaluation', 'factors', 'framework', 'guidelines', 'kanban', 'lean', 'method adaptation', 'method configuration', 'method customization', 'method tailoring', 'methodology', 'metrics', 'practical', 'process', 'scrum']</t>
         </is>
       </c>
       <c r="Q17" t="n">
@@ -1663,7 +1675,7 @@
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
-          <t>("agile practice*" OR "agile method*" OR scrum OR kanban) AND ("critical success factor*" OR CSF) AND ("global software development" OR GSD OR "distributed software development") AND ("green software" OR "sustainable software" OR "green IT" OR "sustainable IT")</t>
+          <t>("Agile practices" OR Scrum OR Kanban OR XP OR "Agile methodologies") AND ("Critical Success Factors" OR "success factors" OR "key success factors" OR "critical factors") AND (GSD OR "offshore software development" OR "distributed software development" OR outsourcing) AND ("green and sustainable software" OR "sustainable software" OR "green software" OR "eco-friendly software" OR "energy-efficient software")</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -1673,7 +1685,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>['agile method*', 'agile practice*', 'critical success factor*', 'csf', 'distributed software development', 'global software development', 'green it', 'green software', 'gsd', 'kanban', 'scrum', 'sustainable it', 'sustainable software']</t>
+          <t>['agile methodologies', 'agile practices', 'critical factors', 'critical success factors', 'distributed software development', 'eco-friendly software', 'energy-efficient software', 'green', 'green software', 'gsd', 'kanban', 'key success factors', 'offshore software development', 'outsourcing', 'scrum', 'success factors', 'sustainable software', 'sustainable software', 'xp']</t>
         </is>
       </c>
       <c r="Q18" t="n">
@@ -1730,7 +1742,7 @@
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
-          <t>("CMMI-DEV" OR "Capability Maturity Model Integration") AND (Agile OR Scrum OR Kanban OR "Extreme Programming") AND (Web OR "Web-based" OR "Web environment" OR "Web application") AND ("maturity level*" OR "process area*") AND ("evaluation criteria" OR "validation" OR "experiment*" OR "case study")</t>
+          <t>("CMMI-DEV" OR "CMMI" OR "Capability Maturity Model Integration" OR "maturity models") AND ("Agile methodologies" OR "Agile methods" OR "Scrum" OR "XP" OR "Kanban" OR "Agile development") AND ("Web environments" OR "Web applications" OR "Web development" OR "Web-based") AND ("maturity levels" OR "maturity assessment") AND ("evaluation criteria" OR "evaluation methods" OR "assessment criteria") AND ("experiments" OR "case studies" OR "empirical studies") AND ("validation" OR "verification") AND ("Web specific characteristics")</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
@@ -1740,11 +1752,11 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>['agile', 'capability maturity model integration', 'case study', 'cmmi-dev', 'evaluation criteria', 'experiment*', 'extreme programming', 'kanban', 'maturity level*', 'process area*', 'scrum', 'validation', 'web', 'web application', 'web environment', 'web-based']</t>
+          <t>['agile development', 'agile methodologies', 'agile methods', 'assessment criteria', 'capability maturity model integration', 'case studies', 'cmmi', 'cmmi-dev', 'empirical studies', 'evaluation criteria', 'evaluation methods', 'experiments', 'kanban', 'maturity assessment', 'maturity levels', 'maturity models', 'scrum', 'validation', 'verification', 'web applications', 'web development', 'web environments', 'web specific characteristics', 'web-based', 'xp']</t>
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>0.2</v>
+        <v>0.06451612903225806</v>
       </c>
     </row>
     <row r="20">
@@ -1791,7 +1803,11 @@
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>("data collection methods" OR "data gathering techniques" OR "survey methods" OR "interview methods" OR "case studies") AND ("curriculum models" OR "bodies of knowledge" OR "software engineering education" OR "SE curriculum design") AND (("SE skills" OR "software engineering skills" OR "technical skills" OR "programming skills" OR "software design skills") AND ("importance" OR "deficiencies" OR "knowledge gaps" OR "skill gaps")) AND ("soft skills" OR "non-technical skills" OR "communication skills" OR "teamwork skills" OR "interpersonal skills") AND ("hard skills" OR "technical skills") AND ("data sample" OR "participant demographics" OR "study population" OR "sample size") AND ("regional coverage" OR "geographic distribution" OR "countries") AND ("educational recommendations" OR "curriculum improvement" OR "teaching methods") AND ("meta-analysis" OR "literature review" OR "systematic review") AND ("software engineer" OR "software developers" OR "programmers")</t>
+        </is>
+      </c>
       <c r="O20" t="inlineStr">
         <is>
           <t>['desired skills', 'educational needs', 'essential competencies', 'knowledge needs', 'knowledge requirements', 'skill requirements', 'software developers', 'software engineers']</t>
@@ -1799,11 +1815,11 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>['nan']</t>
+          <t>['bodies of knowledge', 'case studies', 'communication skills', 'countries', 'curriculum improvement', 'curriculum models', 'data collection methods', 'data gathering techniques', 'data sample', 'deficiencies', 'educational recommendations', 'geographic distribution', 'hard skills', 'importance', 'interpersonal skills', 'interview methods', 'knowledge gaps', 'literature review', 'meta-analysis', 'non-technical skills', 'participant demographics', 'programmers', 'programming skills', 'regional coverage', 'sample size', 'se curriculum design', 'se skills', 'skill gaps', 'soft skills', 'software design skills', 'software developers', 'software engineer', 'software engineering education', 'software engineering skills', 'study population', 'survey methods', 'systematic review', 'teaching methods', 'teamwork skills', 'technical skills', 'technical skills']</t>
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>0.02127659574468085</v>
       </c>
     </row>
     <row r="21">
@@ -1856,7 +1872,7 @@
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
-          <t>("app review analysis" OR "application review analysis" OR "user feedback analysis" OR "sentiment analysis" OR "text mining") AND (techniques OR methods OR approaches OR algorithms) AND (software engineering OR software development OR requirements engineering OR maintenance OR testing) AND (empirical evaluation OR validation OR case study OR experiment) AND (effectiveness OR performance OR support OR impact)</t>
+          <t>("app review analysis" OR "application review analysis" OR "user feedback analysis" OR "sentiment analysis" OR "opinion mining" OR "app reviews" OR "reviews analysis") AND ("techniques" OR "methods" OR "approaches" OR "algorithms" OR "natural language processing" OR "machine learning") AND ("software engineering activities" OR "software development" OR "requirements engineering" OR "testing" OR "maintenance" OR "evolution" OR "software engineers" OR "engineering activities") AND ("empirical evaluation" OR "experiments" OR "case studies" OR "user studies" OR "performance evaluation" OR "empirically evaluated" OR "evaluation methods")</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -1866,7 +1882,7 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>['algorithms', 'app review analysis', 'application review analysis', 'approaches', 'case study', 'effectiveness', 'empirical evaluation', 'experiment', 'impact', 'maintenance', 'methods', 'performance', 'requirements engineering', 'sentiment analysis', 'software development', 'software engineering', 'support', 'techniques', 'testing', 'text mining', 'user feedback analysis', 'validation']</t>
+          <t>['algorithms', 'app review analysis', 'app reviews', 'application review analysis', 'approaches', 'case studies', 'empirical evaluation', 'empirically evaluated', 'engineering activities', 'evaluation methods', 'evolution', 'experiments', 'machine learning', 'maintenance', 'methods', 'natural language processing', 'opinion mining', 'performance evaluation', 'requirements engineering', 'reviews analysis', 'sentiment analysis', 'software development', 'software engineering activities', 'software engineers', 'techniques', 'testing', 'user feedback analysis', 'user studies']</t>
         </is>
       </c>
       <c r="Q21" t="n">
@@ -1920,7 +1936,7 @@
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
-          <t>("offshore development" OR "offshore outsourcing") AND (vendor OR "service provider") AND (reliability OR "service quality" OR dependability) AND (challenges OR issues OR risks OR problems) AND (impact OR effect) AND (client OR customer) AND (prioritization OR "risk assessment" OR "value allocation" OR categorization OR "critical issues")</t>
+          <t>("offshore development outsourcing" OR "offshore software development" OR "outsourcing development" OR "outsourcing services") AND ("vendor organization" OR "outsourcing vendors" OR "service providers") AND (reliability OR trustworthiness OR dependability) AND (challenges OR issues OR problems OR difficulties OR barriers OR risks OR failures) AND ("value allocation" OR prioritization OR categorization)</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
@@ -1930,7 +1946,7 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>['categorization', 'challenges', 'client', 'critical issues', 'customer', 'dependability', 'effect', 'impact', 'issues', 'offshore development', 'offshore outsourcing', 'prioritization', 'problems', 'reliability', 'risk assessment', 'risks', 'service provider', 'service quality', 'value allocation', 'vendor']</t>
+          <t>['barriers', 'categorization', 'challenges', 'dependability', 'difficulties', 'failures', 'issues', 'offshore development outsourcing', 'offshore software development', 'outsourcing development', 'outsourcing services', 'outsourcing vendors', 'prioritization', 'problems', 'reliability', 'risks', 'service providers', 'trustworthiness', 'value allocation', 'vendor organization']</t>
         </is>
       </c>
       <c r="Q22" t="n">
@@ -1983,7 +1999,7 @@
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
         <is>
-          <t>("software testing" OR "testing domain") AND (ontology OR ontologies) AND (concept OR concepts OR relationship OR relationships OR property OR properties OR axiom OR axioms) AND (classification OR classified OR categorization OR categorized)</t>
+          <t>("ontology" OR "ontologies" OR "ontology-based" OR "conceptual model" OR "knowledge representation" OR "domain model" OR "taxonomy") AND ("software testing" OR "software test" OR "testing of software" OR "test automation" OR "test design" OR "test case generation" OR "software verification") AND ("classification" OR "categorization")</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -1993,11 +2009,11 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>['axiom', 'axioms', 'categorization', 'categorized', 'classification', 'classified', 'concept', 'concepts', 'ontologies', 'ontology', 'properties', 'property', 'relationship', 'relationships', 'software testing', 'testing domain']</t>
+          <t>['categorization', 'classification', 'conceptual model', 'domain model', 'knowledge representation', 'ontologies', 'ontology', 'ontology-based', 'software test', 'software testing', 'software verification', 'taxonomy', 'test automation', 'test case generation', 'test design', 'testing of software']</t>
         </is>
       </c>
       <c r="Q23" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="24">
@@ -2048,7 +2064,11 @@
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>("experience curve" OR "learning curve" OR "progress function" OR "experience effects" OR "learning effects") AND ("software engineering" OR "software development" OR "software design" OR "programming" OR "software lifecycle" OR "requirements" OR "design" OR "implementation" OR "testing" OR "maintenance")</t>
+        </is>
+      </c>
       <c r="O24" t="inlineStr">
         <is>
           <t>['“experience curve”', '“learning curve”', '“software development”', '“software engineering”', '“software process”', '“software project”']</t>
@@ -2056,7 +2076,7 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>['nan']</t>
+          <t>['design', 'experience curve', 'experience effects', 'implementation', 'learning curve', 'learning effects', 'maintenance', 'programming', 'progress function', 'requirements', 'software design', 'software development', 'software engineering', 'software lifecycle', 'testing']</t>
         </is>
       </c>
       <c r="Q24" t="n">
@@ -2110,7 +2130,7 @@
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr">
         <is>
-          <t>("IT personnel" OR "information technology staff" OR "computer professionals" OR "IT employees") AND ("intentions to leave" OR "turnover intention" OR "employee attrition" OR "job abandonment" OR "resignation") AND (drivers OR factors OR reasons OR motivations OR causes OR predictors OR determinants) AND (workplace OR organization OR company OR employment)</t>
+          <t>("IT personnel" OR "information technology staff" OR "computer professionals" OR "IT employees") AND ("intention to leave" OR "employee turnover" OR "attrition" OR "job abandonment" OR "resignation" OR "turnover intention") AND ("job satisfaction" OR "organizational commitment" OR "work environment" OR "employee engagement" OR "burnout")</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
@@ -2120,7 +2140,7 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>['causes', 'company', 'computer professionals', 'determinants', 'drivers', 'employee attrition', 'employment', 'factors', 'information technology staff', 'intentions to leave', 'it employees', 'it personnel', 'job abandonment', 'motivations', 'organization', 'predictors', 'reasons', 'resignation', 'turnover intention', 'workplace']</t>
+          <t>['attrition', 'burnout', 'computer professionals', 'employee engagement', 'employee turnover', 'information technology staff', 'intention to leave', 'it employees', 'it personnel', 'job abandonment', 'job satisfaction', 'organizational commitment', 'resignation', 'turnover intention', 'work environment']</t>
         </is>
       </c>
       <c r="Q25" t="n">
@@ -2180,7 +2200,11 @@
           <t>An essential requirement is the integration of user experience methods in Agile software development. Based on this, the development of positive user experience must be managed. We understand management in general as a combination of a goal, a strategy, and resources. When applied to UX, user experience management consists of a UX goal, a UX strategy, and UX resources.</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>("Agile software development" OR "Agile development" OR Scrum OR Kanban) AND ("user experience" OR UX OR "user-centered design" OR UCD OR usability) AND (management OR planning OR control OR strategy OR resources) AND ("product backlog" OR requirement OR "user story") AND (retrospective OR improvement OR efficiency OR effectiveness) AND ("software engineering" OR software OR engineering OR "software design" OR "system engineering")</t>
+        </is>
+      </c>
       <c r="O26" t="inlineStr">
         <is>
           <t>['agile', 'hcd', 'hci', 'hmi', 'kanban', 'lean', 'scrum', 'ucd', 'usability', 'ux', '“design thinking”and“user experience”', '“extreme programming”']</t>
@@ -2188,11 +2212,11 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>['nan']</t>
+          <t>['agile development', 'agile software development', 'control', 'effectiveness', 'efficiency', 'engineering', 'improvement', 'kanban', 'management', 'planning', 'product backlog', 'requirement', 'resources', 'retrospective', 'scrum', 'software', 'software design', 'software engineering', 'strategy', 'system engineering', 'ucd', 'usability', 'user experience', 'user story', 'user-centered design', 'ux']</t>
         </is>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>0.1515151515151515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scripts to also automate validation and generation of search strings with a followup prompt
</commit_message>
<xml_diff>
--- a/validation/final_paper_selection.xlsx
+++ b/validation/final_paper_selection.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,21 @@
           <t>jaccard_similarity</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>followup_prompt</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>bot_generated_search_string_followup</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>jaccard_scores_followup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -566,7 +581,7 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>("software maintenance" OR "software evolution" OR "legacy systems" OR "technical debt") AND ("globally distributed settings" OR "distributed software development" OR "offshore development" OR "global software engineering") AND ("challenges" OR "difficulties" OR "problems" OR "issues" OR "obstacles") AND ("mitigation strategies" OR "coping mechanisms" OR "solutions" OR "best practices" OR "management strategies")</t>
+          <t>("software maintenance" OR "software evolution" OR "code maintenance" OR "legacy system maintenance") AND ("global software development" OR "distributed software development" OR "offshore software development" OR "outsourced software development" OR "geographically distributed teams") AND ("challenges" OR "difficulties" OR "issues" OR "problems") AND ("mitigation" OR "strategies" OR "solutions" OR "best practices")</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -576,11 +591,20 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>['best practices', 'challenges', 'coping mechanisms', 'difficulties', 'distributed software development', 'global software engineering', 'globally distributed settings', 'issues', 'legacy systems', 'management strategies', 'mitigation strategies', 'obstacles', 'offshore development', 'problems', 'software evolution', 'software maintenance', 'solutions', 'technical debt']</t>
+          <t>['best practices', 'challenges', 'code maintenance', 'difficulties', 'distributed software development', 'geographically distributed teams', 'global software development', 'issues', 'legacy system maintenance', 'mitigation', 'offshore software development', 'outsourced software development', 'problems', 'software evolution', 'software maintenance', 'solutions', 'strategies']</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.06451612903225806</v>
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>(software OR "software maintenance" OR maintenance OR "software evolution" OR evolution OR code OR "code maintenance" OR legacy OR "legacy system" OR "legacy system maintenance") AND (global OR "global software" OR "global software development" OR distributed OR "distributed software" OR "distributed software development" OR offshore OR "offshore software" OR "offshore software development" OR outsourced OR "outsourced software" OR "outsourced software development" OR geographically OR "geographically distributed" OR "geographically distributed teams" OR teams) AND (challenge OR "challenges" OR difficulty OR "difficulties" OR issue OR "issues" OR problem OR "problems") AND (mitigation OR strategy OR "strategies" OR solution OR "solutions" OR "best practice" OR "best practices")</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
+        <v>0.05660377358490566</v>
       </c>
     </row>
     <row r="3">
@@ -635,7 +659,7 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>("Cloud Software Development Optimization" OR "Cloud Software Development" OR "Software Development Optimization" OR CSDO) AND ("success factors" OR "critical success factors" OR "key success factors" OR enablers OR drivers OR determinants) AND (findings OR research OR studies OR literature) AND ("expert perspectives" OR "expert views" OR "industry experts" OR practitioners) AND (prioritization OR ranking OR taxonomy OR classification OR categorization)</t>
+          <t>("Continuous Software Delivery Optimization" OR CSDO) AND ("success factors" OR "critical success factors" OR enablers OR drivers) AND (challenges OR barriers) AND ("literature review" OR "expert opinions" OR "survey findings") AND (prioritization OR taxonomy OR development OR prioritize)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -645,11 +669,20 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>['categorization', 'classification', 'cloud software development', 'cloud software development optimization', 'critical success factors', 'csdo', 'determinants', 'drivers', 'enablers', 'expert perspectives', 'expert views', 'findings', 'industry experts', 'key success factors', 'literature', 'practitioners', 'prioritization', 'ranking', 'research', 'software development optimization', 'studies', 'success factors', 'taxonomy']</t>
+          <t>['barriers', 'challenges', 'continuous software delivery optimization', 'critical success factors', 'csdo', 'development', 'drivers', 'enablers', 'expert opinions', 'literature review', 'prioritization', 'prioritize', 'success factors', 'survey findings', 'taxonomy']</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0.0425531914893617</v>
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>(Continuous AND Software AND Delivery AND Optimization OR "Continuous Software Delivery" OR "Software Delivery Optimization" OR CSDO) AND (success OR factors OR "success factors" OR critical OR "critical success" OR "critical success factors" OR enablers OR drivers) AND (challenges OR barriers) AND (literature OR review OR "literature review" OR expert OR opinions OR "expert opinions" OR survey OR findings OR "survey findings") AND (prioritization OR taxonomy OR development OR prioritize)</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
+        <v>0.05660377358490566</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +731,7 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>("model transformation" OR "metamodeling" OR "transformation languages") AND ("design patterns" OR "pattern application") AND (practice OR "empirical studies" OR "industrial experience") AND (categories OR types) AND (explicit OR implicit) AND (benefits OR advantages) AND ("adoption over time" OR trends)</t>
+          <t>("model transformation" OR MT OR "model-driven transformation") AND ("design pattern" OR "pattern application" OR "pattern usage" OR "pattern implementation") AND ("in practice" OR "real-world" OR "empirical study" OR "case study" OR "industrial experience") AND ("pattern classification" OR "pattern taxonomy") AND ("explicitly used" OR "implicitly used" OR "recognized pattern" OR "unrecognized pattern") AND ("benefits of patterns" OR "advantages of patterns" OR "evidence of benefits" OR "empirical validation") AND ("patterns not applied" OR "should have used patterns" OR "lack of pattern use") AND ("missing patterns" OR "unformalized patterns" OR "patterns not formalized") AND ("pattern adoption trends" OR "changes in pattern use" OR "evolution of patterns") AND ("impact of pattern catalogs" OR "influence of pattern literature" OR "use of pattern books") AND ("MT language comparison" OR "pattern expressiveness" OR "language support for patterns")</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -708,11 +741,20 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>['adoption over time', 'advantages', 'benefits', 'categories', 'design patterns', 'empirical studies', 'explicit', 'implicit', 'industrial experience', 'metamodeling', 'model transformation', 'pattern application', 'practice', 'transformation languages', 'trends', 'types']</t>
+          <t>['advantages of patterns', 'benefits of patterns', 'case study', 'changes in pattern use', 'design pattern', 'empirical study', 'empirical validation', 'evidence of benefits', 'evolution of patterns', 'explicitly used', 'impact of pattern catalogs', 'implicitly used', 'in practice', 'industrial experience', 'influence of pattern literature', 'lack of pattern use', 'language support for patterns', 'missing patterns', 'model transformation', 'model-driven transformation', 'mt', 'mt language comparison', 'pattern adoption trends', 'pattern application', 'pattern classification', 'pattern expressiveness', 'pattern implementation', 'pattern taxonomy', 'pattern usage', 'patterns not applied', 'patterns not formalized', 'real-world', 'recognized pattern', 'should have used patterns', 'unformalized patterns', 'unrecognized pattern', 'use of pattern books']</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>0.0625</v>
+        <v>0.02702702702702703</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>(model transformation OR MT OR "model-driven transformation" OR model OR transformation OR "driven transformation") AND ("design pattern" OR "pattern application" OR "pattern usage" OR "pattern implementation" OR design OR pattern OR application OR usage OR implementation) AND ("in practice" OR "real-world" OR "empirical study" OR "case study" OR "industrial experience" OR practice OR real OR world OR empirical OR study OR case OR industrial OR experience) AND ("pattern classification" OR "pattern taxonomy" OR classification OR taxonomy) AND ("explicitly used" OR "implicitly used" OR "recognized pattern" OR "unrecognized pattern" OR explicitly OR implicitly OR recognized OR unrecognized OR used) AND ("benefits of patterns" OR "advantages of patterns" OR "evidence of benefits" OR "empirical validation" OR benefits OR advantages OR evidence OR empirical OR validation OR patterns) AND ("patterns not applied" OR "should have used patterns" OR "lack of pattern use" OR applied OR lack) AND ("missing patterns" OR "unformalized patterns" OR "patterns not formalized" OR missing OR unformalized OR formalized) AND ("pattern adoption trends" OR "changes in pattern use" OR "evolution of patterns" OR adoption OR trends OR changes OR evolution) AND ("impact of pattern catalogs" OR "influence of pattern literature" OR "use of pattern books" OR impact OR influence OR literature OR catalogs OR books) AND ("MT language comparison" OR "pattern expressiveness" OR "language support for patterns" OR language OR comparison OR expressiveness OR support)</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>0.01204819277108434</v>
       </c>
     </row>
     <row r="5">
@@ -764,7 +806,7 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>("blockchain governance" OR "distributed ledger governance" OR blockchain) AND ("building blocks" OR components OR elements OR framework OR infrastructure OR foundations OR architecture)</t>
+          <t>("blockchain governance" OR "blockchain" OR "distributed ledger technology") AND ("governance" OR "management" OR "regulation" OR "control") AND ("building blocks" OR "components" OR "elements")</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -774,11 +816,20 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>['architecture', 'blockchain', 'blockchain governance', 'building blocks', 'components', 'distributed ledger governance', 'elements', 'foundations', 'framework', 'infrastructure']</t>
+          <t>['blockchain', 'blockchain governance', 'building blocks', 'components', 'control', 'distributed ledger technology', 'elements', 'governance', 'management', 'regulation']</t>
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>(blockchain OR "distributed ledger technology" OR "distributed ledger" OR "DLT" OR "block chain") AND (governance OR management OR regulation OR control OR "corporate governance" OR "IT governance" OR "risk management" OR "compliance") AND ("building blocks" OR components OR elements OR "core components" OR "fundamental elements" OR "basic building blocks")</t>
+        </is>
+      </c>
+      <c r="T5" t="n">
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="6">
@@ -827,7 +878,7 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>("Model Car Racing" OR MCR OR "miniature car racing" OR "radio-controlled car racing") AND ("theory" OR "principles" OR "framework" OR "knowledge base") AND ("method" OR "technique" OR "strategy" OR "support") AND ("evaluation" OR "assessment" OR "validation" OR "conclusion" OR "result" OR "outcome")</t>
+          <t>("model-based code reuse" OR "model driven code reuse" OR "model based software reuse" OR "model driven software reuse" OR "MCR") AND ("foundational knowledge" OR "body of knowledge" OR "underlying principles" OR "theoretical basis") AND ("approach" OR "method" OR "technique" OR "strategy") AND ("evaluation" OR "assessment" OR "validation" OR "testing") AND ("conclusion" OR "result" OR "finding" OR "outcome")</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -837,10 +888,19 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>['assessment', 'conclusion', 'evaluation', 'framework', 'knowledge base', 'mcr', 'method', 'miniature car racing', 'model car racing', 'outcome', 'principles', 'radio-controlled car racing', 'result', 'strategy', 'support', 'technique', 'theory', 'validation']</t>
+          <t>['approach', 'assessment', 'body of knowledge', 'conclusion', 'evaluation', 'finding', 'foundational knowledge', 'mcr', 'method', 'model based software reuse', 'model driven code reuse', 'model driven software reuse', 'model-based code reuse', 'outcome', 'result', 'strategy', 'technique', 'testing', 'theoretical basis', 'underlying principles', 'validation']</t>
         </is>
       </c>
       <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>(model AND based AND code AND reuse OR "model-based code reuse" OR model AND driven AND code AND reuse OR "model driven code reuse" OR model AND based AND software AND reuse OR "model based software reuse" OR model AND driven AND software AND reuse OR "model driven software reuse" OR MCR) AND (foundational AND knowledge OR body AND knowledge OR underlying AND principles OR theoretical AND basis OR "foundational knowledge" OR "body of knowledge" OR "underlying principles" OR "theoretical basis") AND (approach OR method OR technique OR strategy) AND (evaluation OR assessment OR validation OR testing) AND (conclusion OR result OR finding OR outcome)</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -890,7 +950,7 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>("visual notation" OR "visual notations" OR diagram OR diagrams OR model OR models OR "graphical representation" OR "graphical representations") AND ("Physics of Notations" OR "PoN theory" OR "PoN") AND (analysis OR analyzed OR "analyzing") AND ("user requirements" OR "notation user" OR "user experience") AND (verifiable OR verification OR "analysis validity")</t>
+          <t>("visual notation" OR "diagrammatic representation" OR "modeling language" OR UML OR BPMN OR ERD) AND ("Physics of Notations" OR "PoN theory") AND (analysis OR evaluation OR assessment OR validation) AND ("user requirements" OR usability OR "user experience" OR "cognitive aspects") AND (verifiability OR validation OR reliability OR accuracy)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -900,10 +960,19 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>['analysis', 'analysis validity', 'analyzed', 'analyzing', 'diagram', 'diagrams', 'graphical representation', 'graphical representations', 'model', 'models', 'notation user', 'physics of notations', 'pon', 'pon theory', 'user experience', 'user requirements', 'verifiable', 'verification', 'visual notation', 'visual notations']</t>
+          <t>['accuracy', 'analysis', 'assessment', 'bpmn', 'cognitive aspects', 'diagrammatic representation', 'erd', 'evaluation', 'modeling language', 'physics of notations', 'pon theory', 'reliability', 'uml', 'usability', 'user experience', 'user requirements', 'validation', 'validation', 'verifiability', 'visual notation']</t>
         </is>
       </c>
       <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>(visual OR visuals OR notation OR notations OR diagram OR diagrams OR diagrammatic OR representation OR representations OR model OR models OR modeling OR language OR languages OR UML OR BPMN OR ERD) AND (Physics OR Physics of Notations OR Physics of Notation OR PoN OR theory OR theories OR "PoN theory") AND (analysis OR analyses OR evaluation OR evaluations OR assessment OR assessments OR validate OR validates OR validation OR validations) AND (user OR users OR requirement OR requirements OR usability OR usabilities OR experience OR experiences OR "user requirements" OR "user experience" OR cognitive OR cognitives OR aspect OR aspects) AND (verifiability OR verifiable OR validation OR validations OR reliability OR reliable OR accuracy OR accurate)</t>
+        </is>
+      </c>
+      <c r="T7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -953,7 +1022,7 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>("semi-automatic configuration" OR "assisted configuration" OR "partially automated configuration" OR "configuration") AND ("extended product lines" OR "software product lines" OR "SPL" OR "product family") AND (evaluation OR validation OR experiment OR "case study" OR "performance analysis") AND ("open challenges" OR limitations OR "future research" OR "unresolved issues")</t>
+          <t>("semi-automatic configuration" OR "semi automatic configuration") AND ("product lines" OR "product line" OR "PL") AND (evaluation OR assessment OR validation) AND ("open challenges" OR "future research" OR limitations)</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -963,11 +1032,20 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>['assisted configuration', 'case study', 'configuration', 'evaluation', 'experiment', 'extended product lines', 'future research', 'limitations', 'open challenges', 'partially automated configuration', 'performance analysis', 'product family', 'semi-automatic configuration', 'software product lines', 'spl', 'unresolved issues', 'validation']</t>
+          <t>['assessment', 'evaluation', 'future research', 'limitations', 'open challenges', 'pl', 'product line', 'product lines', 'semi automatic configuration', 'semi-automatic configuration', 'validation']</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>0.03703703703703703</v>
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>(("semi-automatic configuration" OR "semi automatic configuration" OR "semi-automatic" OR "semi automatic" OR "configuration")) AND (("product lines" OR "product line" OR "PL" OR "products" OR "lines")) AND ((evaluation OR assessment OR validation OR evaluate OR assess OR validate)) AND (("open challenges" OR "future research" OR limitations OR "open challenge" OR "future" OR "research" OR challenge))</t>
+        </is>
+      </c>
+      <c r="T8" t="n">
+        <v>0.0303030303030303</v>
       </c>
     </row>
     <row r="9">
@@ -1053,7 +1131,7 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>("deep learning" OR "neural networks" OR "machine learning") AND ("software engineering" OR "software development" OR "software design" OR "software maintenance") AND (data OR artifacts) AND (extraction OR preprocessing) AND (model OR architecture OR training) AND (evaluation OR benchmark) AND (reproducibility OR replication)</t>
+          <t>("software engineering" OR "software development" OR "software maintenance" OR "software testing" OR "requirements engineering" OR "software" OR "engineering") AND ("deep learning" OR "neural networks" OR "machine learning" OR CNN OR RNN OR transformer) AND ("software data" OR "code data" OR "data extraction" OR "data preprocessing" OR "feature engineering") AND ("baseline methods" OR benchmarks OR "reproducibility studies" OR "generalization performance")</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1063,10 +1141,19 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>['architecture', 'artifacts', 'benchmark', 'data', 'deep learning', 'evaluation', 'extraction', 'machine learning', 'model', 'neural networks', 'preprocessing', 'replication', 'reproducibility', 'software design', 'software development', 'software engineering', 'software maintenance', 'training']</t>
+          <t>['baseline methods', 'benchmarks', 'cnn', 'code data', 'data extraction', 'data preprocessing', 'deep learning', 'engineering', 'feature engineering', 'generalization performance', 'machine learning', 'neural networks', 'reproducibility studies', 'requirements engineering', 'rnn', 'software', 'software data', 'software development', 'software engineering', 'software maintenance', 'software testing', 'transformer']</t>
         </is>
       </c>
       <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>(software OR engineering OR "software engineering" OR "software development" OR development OR "software maintenance" OR maintenance OR "software testing" OR testing OR "requirements engineering" OR requirements OR "software" OR "engineering") AND (deep OR learning OR "deep learning" OR "neural networks" OR neural OR networks OR "machine learning" OR machine OR learning OR CNN OR RNN OR transformer) AND (software OR data OR "software data" OR "code data" OR code OR data OR "data extraction" OR extraction OR "data preprocessing" OR preprocessing OR "feature engineering" OR feature OR engineering) AND (baseline OR methods OR "baseline methods" OR benchmarks OR "reproducibility studies" OR reproducibility OR studies OR "generalization performance" OR generalization OR performance)</t>
+        </is>
+      </c>
+      <c r="T9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1120,7 +1207,7 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>("software trust" OR "trustworthiness of software" OR "confidence in software") AND (definition OR concept OR understanding) OR ("SECO trust" OR "secure coding trust") AND (definition OR concept OR understanding) OR ("software product selection" OR "software version selection") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users") OR ("software package managers") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users") OR ("software producing organizations") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users") OR ("software engineers") AND ("trust factors" OR "trust indicators" OR "trust metrics" OR "trust evaluation criteria") AND ("end-user organizations" OR "users")</t>
+          <t>("software trust" OR "SECO trust" OR "software security trust") AND (definition OR concept OR factors OR criteria) AND ("software product selection" OR "software package manager selection" OR "software producing organization selection" OR "software engineer selection" OR "software selection") AND ("end-user" OR "organization" OR "company")</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1130,10 +1217,15 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>['concept', 'concept', 'confidence in software', 'definition', 'definition', 'end-user organizations', 'end-user organizations', 'end-user organizations', 'end-user organizations', 'seco trust', 'secure coding trust', 'software engineers', 'software package managers', 'software producing organizations', 'software product selection', 'software trust', 'software version selection', 'trust evaluation criteria', 'trust evaluation criteria', 'trust evaluation criteria', 'trust evaluation criteria', 'trust factors', 'trust factors', 'trust factors', 'trust factors', 'trust indicators', 'trust indicators', 'trust indicators', 'trust indicators', 'trust metrics', 'trust metrics', 'trust metrics', 'trust metrics', 'trustworthiness of software', 'understanding', 'understanding', 'users', 'users', 'users', 'users']</t>
+          <t>['company', 'concept', 'criteria', 'definition', 'end-user', 'factors', 'organization', 'seco trust', 'software engineer selection', 'software package manager selection', 'software producing organization selection', 'software product selection', 'software security trust', 'software selection', 'software trust']</t>
         </is>
       </c>
       <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1181,11 +1273,7 @@
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>("data mining" OR "data analysis" OR "machine learning") AND ("software distribution platform" OR "app store" OR "application store") AND (review OR reviews) AND (usefulness OR helpfulness OR quality) AND ("spam review" OR "fake review" OR "deceptive review") AND (legitimate OR genuine OR authentic) AND ("software feature" OR "application feature" OR "functionality") AND (extraction OR mining OR identification) AND ("domain dependency" OR "context dependency")</t>
-        </is>
-      </c>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
           <t>['analysis', 'app', 'application', 'apps', 'appstore', 'bug', 'comment', 'complain', 'data', 'ecosystem', 'expectation', 'feature', 'helpfulness', 'issue', 'market', 'mining', 'mobile', 'online', 'opinion', 'processing', 'quality', 'rating', 'request', 'requirement', 'review', 'sentiment', 'software', 'store', 'text', 'usefulness', 'user', 'vocabulary']</t>
@@ -1193,11 +1281,16 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>['app store', 'application feature', 'application store', 'authentic', 'context dependency', 'data analysis', 'data mining', 'deceptive review', 'domain dependency', 'extraction', 'fake review', 'functionality', 'genuine', 'helpfulness', 'identification', 'legitimate', 'machine learning', 'mining', 'quality', 'review', 'reviews', 'software distribution platform', 'software feature', 'spam review', 'usefulness']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>0.09615384615384616</v>
+        <v>0</v>
+      </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1246,11 +1339,7 @@
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>("visualization techniques" OR "visual representation" OR "data visualization") AND ("software architecture" OR "architectural design" OR "system architecture" OR "software design") AND ("architecting process" OR "architecting activities" OR "architecture visualization tools" OR "software visualization")</t>
-        </is>
-      </c>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
           <t>['architecting', 'architectural', 'architecture', 'diagram', 'graphic', 'graphical', 'picture', 'structure', 'visual', 'visualization', 'visualize', 'visualizing']</t>
@@ -1258,10 +1347,15 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>['architecting activities', 'architecting process', 'architectural design', 'architecture visualization tools', 'data visualization', 'software architecture', 'software design', 'software visualization', 'system architecture', 'visual representation', 'visualization techniques']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1315,11 +1409,7 @@
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>("Unified Modeling Language" OR UML) AND (consistency OR integrity OR validation) AND ("formal method" OR "non-formal method" OR technique OR language) AND (diagram OR "class diagram" OR "sequence diagram" OR "activity diagram" OR "state diagram" OR "use case diagram") AND ("consistency check*" OR "integrity check*" OR "validation check*" OR "error detection") AND (extend* OR support OR new)</t>
-        </is>
-      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
           <t>['“consistency”', '“consistency”or “model”', '“inconsistency”', '“inconsistency”', '“management”', '“model”']</t>
@@ -1327,10 +1417,15 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>['activity diagram', 'class diagram', 'consistency', 'consistency check*', 'diagram', 'error detection', 'extend*', 'formal method', 'integrity', 'integrity check*', 'language', 'new', 'non-formal method', 'sequence diagram', 'state diagram', 'support', 'technique', 'uml', 'unified modeling language', 'use case diagram', 'validation', 'validation check*']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1391,11 +1486,7 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>("Search Based Software Testing" OR "search-based software testing" OR "search based software testing" OR "optimization-based software testing" OR "search algorithms for software testing") AND ("mutation testing" OR "mutation analysis" OR "mutation operators" OR "mutants") AND ("genetic algorithms" OR "simulated annealing" OR "particle swarm optimization" OR "evolutionary algorithms") AND ("fitness functions" OR "objective functions" OR "evaluation functions") AND ("mutation generation" OR "mutation execution" OR "mutation analysis") AND ("programming languages")</t>
-        </is>
-      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>['ant colony', 'evelutionary', 'genetic algorithms', 'genetic programming', 'heuristic', 'hill-climbing', 'meta-heuristic', 'metaheuristic', 'mutation analysis', 'mutation based test', 'mutation test', 'mutation testing', 'mutation-based test', 'oprimization', 'program mutation', 'search based', 'search-based', 'simulated annealing', 'tabu search']</t>
@@ -1403,11 +1494,16 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>['evaluation functions', 'evolutionary algorithms', 'fitness functions', 'genetic algorithms', 'mutants', 'mutation analysis', 'mutation analysis', 'mutation execution', 'mutation generation', 'mutation operators', 'mutation testing', 'objective functions', 'optimization-based software testing', 'particle swarm optimization', 'programming languages', 'search algorithms for software testing', 'search based software testing', 'search based software testing', 'search-based software testing', 'simulated annealing']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>0.1212121212121212</v>
+        <v>0</v>
+      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1461,11 +1557,7 @@
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>("code smell" OR "code smells" OR "software smell" OR "software smells" OR "bad code smell" OR "poor code quality") AND ("experiment" OR "empirical study") AND ("theme" OR "finding" OR "result") AND ("comparison" OR "convergence")</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>['anti-patternandexperiment', 'controlled', 'disharmony', 'empirical', 'ethnography', 'smell', 'study', 'survey', '“action research”', '“code anomaly”', '“design anomaly”', '“design flaw”', '“exploratory analysis”']</t>
@@ -1473,10 +1565,15 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>['bad code smell', 'code smell', 'code smells', 'comparison', 'convergence', 'empirical study', 'experiment', 'finding', 'poor code quality', 'result', 'software smell', 'software smells', 'theme']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1525,11 +1622,7 @@
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>("socially intelligent agent*" OR "social agent*" OR "intelligent agent*" OR SIA) AND (input* OR "data source*" OR "information source*" OR feed*) AND (process* OR method* OR technique* OR algorithm*) AND (output* OR result* OR outcome* OR product*) AND (usability OR "ease of use" OR "user experience" OR UX OR accessibility OR acceptance)</t>
-        </is>
-      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>['existing systems', 'legacy', 'migration', 'modernization', 'object-oriented', 're-engineering', 'service identification', 'service mining', 'service packaging', 'transformation']</t>
@@ -1537,10 +1630,15 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>['acceptance', 'accessibility', 'algorithm*', 'data source*', 'ease of use', 'feed*', 'information source*', 'input*', 'intelligent agent*', 'method*', 'outcome*', 'output*', 'process*', 'product*', 'result*', 'sia', 'social agent*', 'socially intelligent agent*', 'technique*', 'usability', 'user experience', 'ux']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1609,11 +1707,7 @@
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>("agile method" OR "agile methods" OR "scrum" OR "kanban" OR "lean") AND ("method tailoring" OR "method adaptation" OR "method customization" OR "method configuration") AND ("methodology" OR "approach" OR "framework" OR "process") AND ("practical" OR "empirical" OR "evaluation" OR "application") AND ("criteria" OR "factors" OR "metrics" OR "guidelines")</t>
-        </is>
-      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
           <t>['adoption orfdd', 'adoption orkanban', 'adoption orlean', 'adoption orscrum', 'adoption orxp', 'adoption or“feature driven development”', 'agile', 'method', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'select', 'select oragile', 'select orfdd', 'select orkanban', 'select orlean', 'select orxp', 'select or“feature driven development”', 'tailoring orfdd', 'tailoring orkanban', 'tailoring orlean', 'tailoring orscrum', 'tailoring orscrum', 'tailoring orxp', 'tailoring or“feature driven development”']</t>
@@ -1621,10 +1715,15 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>['agile method', 'agile methods', 'application', 'approach', 'criteria', 'empirical', 'evaluation', 'factors', 'framework', 'guidelines', 'kanban', 'lean', 'method adaptation', 'method configuration', 'method customization', 'method tailoring', 'methodology', 'metrics', 'practical', 'process', 'scrum']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1673,11 +1772,7 @@
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>("Agile practices" OR Scrum OR Kanban OR XP OR "Agile methodologies") AND ("Critical Success Factors" OR "success factors" OR "key success factors" OR "critical factors") AND (GSD OR "offshore software development" OR "distributed software development" OR outsourcing) AND ("green and sustainable software" OR "sustainable software" OR "green software" OR "eco-friendly software" OR "energy-efficient software")</t>
-        </is>
-      </c>
+      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
           <t>['“agile methods”', '“agile”', '“green agile”', '“green software engineering”', '“green software”', '“greener software”', '“practices”', '“solutions”', '“sustainable software”']</t>
@@ -1685,10 +1780,15 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>['agile methodologies', 'agile practices', 'critical factors', 'critical success factors', 'distributed software development', 'eco-friendly software', 'energy-efficient software', 'green', 'green software', 'gsd', 'kanban', 'key success factors', 'offshore software development', 'outsourcing', 'scrum', 'success factors', 'sustainable software', 'sustainable software', 'xp']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1740,11 +1840,7 @@
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>("CMMI-DEV" OR "CMMI" OR "Capability Maturity Model Integration" OR "maturity models") AND ("Agile methodologies" OR "Agile methods" OR "Scrum" OR "XP" OR "Kanban" OR "Agile development") AND ("Web environments" OR "Web applications" OR "Web development" OR "Web-based") AND ("maturity levels" OR "maturity assessment") AND ("evaluation criteria" OR "evaluation methods" OR "assessment criteria") AND ("experiments" OR "case studies" OR "empirical studies") AND ("validation" OR "verification") AND ("Web specific characteristics")</t>
-        </is>
-      </c>
+      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
           <t>['agile', 'agility', 'capability maturity model', 'cmmi', 'extreme programming', 'scrum', 'web', 'web engineering']</t>
@@ -1752,11 +1848,16 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>['agile development', 'agile methodologies', 'agile methods', 'assessment criteria', 'capability maturity model integration', 'case studies', 'cmmi', 'cmmi-dev', 'empirical studies', 'evaluation criteria', 'evaluation methods', 'experiments', 'kanban', 'maturity assessment', 'maturity levels', 'maturity models', 'scrum', 'validation', 'verification', 'web applications', 'web development', 'web environments', 'web specific characteristics', 'web-based', 'xp']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>0.06451612903225806</v>
+        <v>0</v>
+      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1803,11 +1904,7 @@
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>("data collection methods" OR "data gathering techniques" OR "survey methods" OR "interview methods" OR "case studies") AND ("curriculum models" OR "bodies of knowledge" OR "software engineering education" OR "SE curriculum design") AND (("SE skills" OR "software engineering skills" OR "technical skills" OR "programming skills" OR "software design skills") AND ("importance" OR "deficiencies" OR "knowledge gaps" OR "skill gaps")) AND ("soft skills" OR "non-technical skills" OR "communication skills" OR "teamwork skills" OR "interpersonal skills") AND ("hard skills" OR "technical skills") AND ("data sample" OR "participant demographics" OR "study population" OR "sample size") AND ("regional coverage" OR "geographic distribution" OR "countries") AND ("educational recommendations" OR "curriculum improvement" OR "teaching methods") AND ("meta-analysis" OR "literature review" OR "systematic review") AND ("software engineer" OR "software developers" OR "programmers")</t>
-        </is>
-      </c>
+      <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
           <t>['desired skills', 'educational needs', 'essential competencies', 'knowledge needs', 'knowledge requirements', 'skill requirements', 'software developers', 'software engineers']</t>
@@ -1815,11 +1912,16 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>['bodies of knowledge', 'case studies', 'communication skills', 'countries', 'curriculum improvement', 'curriculum models', 'data collection methods', 'data gathering techniques', 'data sample', 'deficiencies', 'educational recommendations', 'geographic distribution', 'hard skills', 'importance', 'interpersonal skills', 'interview methods', 'knowledge gaps', 'literature review', 'meta-analysis', 'non-technical skills', 'participant demographics', 'programmers', 'programming skills', 'regional coverage', 'sample size', 'se curriculum design', 'se skills', 'skill gaps', 'soft skills', 'software design skills', 'software developers', 'software engineer', 'software engineering education', 'software engineering skills', 'study population', 'survey methods', 'systematic review', 'teaching methods', 'teamwork skills', 'technical skills', 'technical skills']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>0.02127659574468085</v>
+        <v>0</v>
+      </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1870,11 +1972,7 @@
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>("app review analysis" OR "application review analysis" OR "user feedback analysis" OR "sentiment analysis" OR "opinion mining" OR "app reviews" OR "reviews analysis") AND ("techniques" OR "methods" OR "approaches" OR "algorithms" OR "natural language processing" OR "machine learning") AND ("software engineering activities" OR "software development" OR "requirements engineering" OR "testing" OR "maintenance" OR "evolution" OR "software engineers" OR "engineering activities") AND ("empirical evaluation" OR "experiments" OR "case studies" OR "user studies" OR "performance evaluation" OR "empirically evaluated" OR "evaluation methods")</t>
-        </is>
-      </c>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
           <t>["'app review'", "'app store review'", "'app store'", "'requirement engineering'", "'software coding'", "'software configuration'", "'software construction'", "'software design'", "'software development'", "'software engineering'", "'software maintenance'", "'software quality'", "'software requirement'", "'software testing'", "'user feedback'", "'user review'"]</t>
@@ -1882,10 +1980,15 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>['algorithms', 'app review analysis', 'app reviews', 'application review analysis', 'approaches', 'case studies', 'empirical evaluation', 'empirically evaluated', 'engineering activities', 'evaluation methods', 'evolution', 'experiments', 'machine learning', 'maintenance', 'methods', 'natural language processing', 'opinion mining', 'performance evaluation', 'requirements engineering', 'reviews analysis', 'sentiment analysis', 'software development', 'software engineering activities', 'software engineers', 'techniques', 'testing', 'user feedback analysis', 'user studies']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1934,11 +2037,7 @@
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>("offshore development outsourcing" OR "offshore software development" OR "outsourcing development" OR "outsourcing services") AND ("vendor organization" OR "outsourcing vendors" OR "service providers") AND (reliability OR trustworthiness OR dependability) AND (challenges OR issues OR problems OR difficulties OR barriers OR risks OR failures) AND ("value allocation" OR prioritization OR categorization)</t>
-        </is>
-      </c>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
           <t>['dealer', 'developer', 'marketer', 'merchant', 'retailer', 'salesperson', 'seller', 'service-provider', 'trader', 'wholesaler”', '“barriers”', '“challenges”', '“critical factors”', '“global software development”', '“hurdles”', '“issues”', '“obstacles”', '“risk analysis”', '“risks”', '“software outsourcing development”', '“software outsourcing”', '“vendor']</t>
@@ -1946,10 +2045,15 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>['barriers', 'categorization', 'challenges', 'dependability', 'difficulties', 'failures', 'issues', 'offshore development outsourcing', 'offshore software development', 'outsourcing development', 'outsourcing services', 'outsourcing vendors', 'prioritization', 'problems', 'reliability', 'risks', 'service providers', 'trustworthiness', 'value allocation', 'vendor organization']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1997,11 +2101,7 @@
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>("ontology" OR "ontologies" OR "ontology-based" OR "conceptual model" OR "knowledge representation" OR "domain model" OR "taxonomy") AND ("software testing" OR "software test" OR "testing of software" OR "test automation" OR "test design" OR "test case generation" OR "software verification") AND ("classification" OR "categorization")</t>
-        </is>
-      </c>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
           <t>['ontologies', 'ontology', 'software test', 'software testing']</t>
@@ -2009,11 +2109,16 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>['categorization', 'classification', 'conceptual model', 'domain model', 'knowledge representation', 'ontologies', 'ontology', 'ontology-based', 'software test', 'software testing', 'software verification', 'taxonomy', 'test automation', 'test case generation', 'test design', 'testing of software']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q23" t="n">
-        <v>0.25</v>
+        <v>0</v>
+      </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2064,11 +2169,7 @@
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>("experience curve" OR "learning curve" OR "progress function" OR "experience effects" OR "learning effects") AND ("software engineering" OR "software development" OR "software design" OR "programming" OR "software lifecycle" OR "requirements" OR "design" OR "implementation" OR "testing" OR "maintenance")</t>
-        </is>
-      </c>
+      <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr">
         <is>
           <t>['“experience curve”', '“learning curve”', '“software development”', '“software engineering”', '“software process”', '“software project”']</t>
@@ -2076,10 +2177,15 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>['design', 'experience curve', 'experience effects', 'implementation', 'learning curve', 'learning effects', 'maintenance', 'programming', 'progress function', 'requirements', 'software design', 'software development', 'software engineering', 'software lifecycle', 'testing']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2128,11 +2234,7 @@
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>("IT personnel" OR "information technology staff" OR "computer professionals" OR "IT employees") AND ("intention to leave" OR "employee turnover" OR "attrition" OR "job abandonment" OR "resignation" OR "turnover intention") AND ("job satisfaction" OR "organizational commitment" OR "work environment" OR "employee engagement" OR "burnout")</t>
-        </is>
-      </c>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
           <t>['“employee retention”', '“employees retention”', '“intention for turnover”', '“intention to leave”', '“intention to quit”', '“intention to stay”', '“intention to withdraw”', '“is employee”', '“is manager”', '“is personnel”', '“is professional”', '“is workforce”', '“it employee”', '“it manager”', '“it personnel”', '“it professional”', '“it worker”', '“it workforce”', '“leave intention”', '“manager retention”', '“managers retention”', '“personnel retention”', '“professional retention”', '“professionals retention”and “is worker”', '“quit intention”', '“software designer”', '“software developer”', '“software engineer”', '“software manager”', '“software programmer”', '“software project manager”', '“stay intention”', '“system analyst”', '“turnover intention”', '“withdrawal intention”', '“worker retention”', '“workers retention”']</t>
@@ -2140,10 +2242,15 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>['attrition', 'burnout', 'computer professionals', 'employee engagement', 'employee turnover', 'information technology staff', 'intention to leave', 'it employees', 'it personnel', 'job abandonment', 'job satisfaction', 'organizational commitment', 'resignation', 'turnover intention', 'work environment']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2200,11 +2307,7 @@
           <t>An essential requirement is the integration of user experience methods in Agile software development. Based on this, the development of positive user experience must be managed. We understand management in general as a combination of a goal, a strategy, and resources. When applied to UX, user experience management consists of a UX goal, a UX strategy, and UX resources.</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>("Agile software development" OR "Agile development" OR Scrum OR Kanban) AND ("user experience" OR UX OR "user-centered design" OR UCD OR usability) AND (management OR planning OR control OR strategy OR resources) AND ("product backlog" OR requirement OR "user story") AND (retrospective OR improvement OR efficiency OR effectiveness) AND ("software engineering" OR software OR engineering OR "software design" OR "system engineering")</t>
-        </is>
-      </c>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
           <t>['agile', 'hcd', 'hci', 'hmi', 'kanban', 'lean', 'scrum', 'ucd', 'usability', 'ux', '“design thinking”and“user experience”', '“extreme programming”']</t>
@@ -2212,11 +2315,16 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>['agile development', 'agile software development', 'control', 'effectiveness', 'efficiency', 'engineering', 'improvement', 'kanban', 'management', 'planning', 'product backlog', 'requirement', 'resources', 'retrospective', 'scrum', 'software', 'software design', 'software engineering', 'strategy', 'system engineering', 'ucd', 'usability', 'user experience', 'user story', 'user-centered design', 'ux']</t>
+          <t>['nan']</t>
         </is>
       </c>
       <c r="Q26" t="n">
-        <v>0.1515151515151515</v>
+        <v>0</v>
+      </c>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated git ignore. and validation data. script takes like 2 mins to run with 25 data entries
</commit_message>
<xml_diff>
--- a/validation/final_paper_selection.xlsx
+++ b/validation/final_paper_selection.xlsx
@@ -506,27 +506,27 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>followup_prompt</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>bot_generated_search_string_followup</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>ss_words</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>bot_gen_ss_words</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>jaccard_similarity</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>followup_prompt</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>bot_generated_search_string_followup</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
@@ -581,30 +581,30 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>("software maintenance" OR "software evolution" OR "code maintenance" OR "legacy system maintenance") AND ("global software development" OR "distributed software development" OR "offshore software development" OR "outsourced software development" OR "geographically distributed teams") AND ("challenges" OR "difficulties" OR "issues" OR "problems") AND ("mitigation" OR "strategies" OR "solutions" OR "best practices")</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+          <t>("software maintenance" OR "software evolution" OR "software support" OR "legacy systems") AND ("globally distributed settings" OR "global software development" OR "offshore development" OR "distributed teams") AND (challenges OR difficulties OR issues OR problems) AND (mitigation OR strategies OR solutions OR approaches)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>(software OR maintenance OR evolution OR support OR legacy OR systems OR "software maintenance" OR "software evolution" OR "software support" OR "legacy systems") AND (globally OR distributed OR settings OR global OR software OR development OR offshore OR teams OR "globally distributed settings" OR "global software development" OR "offshore development" OR "distributed teams") AND (challenges OR difficulties OR issues OR problems) AND (mitigation OR strategies OR solutions OR approaches)</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>['change', 'distributed software development', 'distributed software engineering', 'distributed software project', 'global enterprise resource planning erp software', 'global enterprise resource planning software', 'global software development', 'global software engineering', 'global software project', 'maintain', 'maintenance', 'software offshore', 'software outsource', 'support', 'upgrade']</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>['best practices', 'challenges', 'code maintenance', 'difficulties', 'distributed software development', 'geographically distributed teams', 'global software development', 'issues', 'legacy system maintenance', 'mitigation', 'offshore software development', 'outsourced software development', 'problems', 'software evolution', 'software maintenance', 'solutions', 'strategies']</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.06666666666666667</v>
-      </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>(software OR "software maintenance" OR maintenance OR "software evolution" OR evolution OR code OR "code maintenance" OR legacy OR "legacy system" OR "legacy system maintenance") AND (global OR "global software" OR "global software development" OR distributed OR "distributed software" OR "distributed software development" OR offshore OR "offshore software" OR "offshore software development" OR outsourced OR "outsourced software" OR "outsourced software development" OR geographically OR "geographically distributed" OR "geographically distributed teams" OR teams) AND (challenge OR "challenges" OR difficulty OR "difficulties" OR issue OR "issues" OR problem OR "problems") AND (mitigation OR strategy OR "strategies" OR solution OR "solutions" OR "best practice" OR "best practices")</t>
-        </is>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>['approaches', 'challenges', 'difficulties', 'distributed teams', 'global software development', 'globally distributed settings', 'issues', 'legacy systems', 'mitigation', 'offshore development', 'problems', 'software evolution', 'software maintenance', 'software support', 'solutions', 'strategies']</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>0.03333333333333333</v>
       </c>
       <c r="T2" t="n">
-        <v>0.05660377358490566</v>
+        <v>0.07317073170731707</v>
       </c>
     </row>
     <row r="3">
@@ -659,30 +659,30 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>("Continuous Software Delivery Optimization" OR CSDO) AND ("success factors" OR "critical success factors" OR enablers OR drivers) AND (challenges OR barriers) AND ("literature review" OR "expert opinions" OR "survey findings") AND (prioritization OR taxonomy OR development OR prioritize)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
+          <t>("Chief Data Officer" OR CSDO) AND ("success factors" OR "critical success factors" OR "key success factors") AND (literature OR "expert opinions" OR "survey findings") AND (prioritization OR taxonomy)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>(Chief OR Data OR Officer OR "Chief Data Officer" OR CSDO) AND (success OR factors OR "success factors" OR "critical success factors" OR critical OR "key success factors" OR key) AND (literature OR "expert opinions" OR expert OR opinions OR "survey findings" OR survey OR findings) AND (prioritization OR taxonomy)</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>['application service', 'asp"and"cloud computing', 'aspects', 'cloud offering', 'cloud platform', 'cloud provider', 'cloud service', 'collaborative software development"and"iaas', 'drivers', 'elements', 'factors', 'geographically distributed development', 'global software development', 'infrastructure as a service', 'it service', 'items', 'motivators', 'multisite development', 'offshore development', 'paas', 'platform as a service', 'saas', 'software as a service', 'success factors', 'variables"and"outsourcing', 'xaas']</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>['barriers', 'challenges', 'continuous software delivery optimization', 'critical success factors', 'csdo', 'development', 'drivers', 'enablers', 'expert opinions', 'literature review', 'prioritization', 'prioritize', 'success factors', 'survey findings', 'taxonomy']</t>
-        </is>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.05128205128205128</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>(Continuous AND Software AND Delivery AND Optimization OR "Continuous Software Delivery" OR "Software Delivery Optimization" OR CSDO) AND (success OR factors OR "success factors" OR critical OR "critical success" OR "critical success factors" OR enablers OR drivers) AND (challenges OR barriers) AND (literature OR review OR "literature review" OR expert OR opinions OR "expert opinions" OR survey OR findings OR "survey findings") AND (prioritization OR taxonomy OR development OR prioritize)</t>
-        </is>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>['chief data officer', 'critical success factors', 'csdo', 'expert opinions', 'key success factors', 'literature', 'prioritization', 'success factors', 'survey findings', 'taxonomy']</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>0.02857142857142857</v>
       </c>
       <c r="T3" t="n">
-        <v>0.05660377358490566</v>
+        <v>0.04444444444444445</v>
       </c>
     </row>
     <row r="4">
@@ -731,30 +731,30 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>("model transformation" OR MT OR "model-driven transformation") AND ("design pattern" OR "pattern application" OR "pattern usage" OR "pattern implementation") AND ("in practice" OR "real-world" OR "empirical study" OR "case study" OR "industrial experience") AND ("pattern classification" OR "pattern taxonomy") AND ("explicitly used" OR "implicitly used" OR "recognized pattern" OR "unrecognized pattern") AND ("benefits of patterns" OR "advantages of patterns" OR "evidence of benefits" OR "empirical validation") AND ("patterns not applied" OR "should have used patterns" OR "lack of pattern use") AND ("missing patterns" OR "unformalized patterns" OR "patterns not formalized") AND ("pattern adoption trends" OR "changes in pattern use" OR "evolution of patterns") AND ("impact of pattern catalogs" OR "influence of pattern literature" OR "use of pattern books") AND ("MT language comparison" OR "pattern expressiveness" OR "language support for patterns")</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
+          <t>("Model Transformation" OR "MT" OR "Model-Driven Transformation" OR "Model Driven Architecture" OR "MDA") AND ("Design Patterns" OR "Architectural Patterns" OR "Software Patterns") AND (Practice OR "Real-world" OR Empirical OR Adoption) AND (Categories OR Types OR "Pattern Classification") AND (Explicit OR Implicit OR Recognized) AND (Benefits OR Advantages OR "Positive Outcomes" OR Effectiveness) AND (Evidence OR Validation OR Empirical Support) AND ("Missed Opportunities" OR "Unapplied Patterns") AND (Formalization OR Standardization) AND ("Adoption Over Time" OR Trends OR Evolution) AND (Influence OR Impact OR "Cited Papers") AND (Languages OR "Transformation Languages" OR "DSL")</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>(Model OR Transformation OR "Model Transformation" OR MT OR "Model-Driven Transformation" OR "Model Driven Architecture" OR MDA OR Driven OR Architecture) AND (Design OR Patterns OR "Design Patterns" OR Architectural OR "Architectural Patterns" OR Software OR "Software Patterns") AND (Practice OR "Real-world" OR Real OR World OR Empirical OR Adoption) AND (Categories OR Types OR "Pattern Classification" OR Pattern OR Classification) AND (Explicit OR Implicit OR Recognized) AND (Benefits OR Advantages OR "Positive Outcomes" OR Positive OR Outcomes OR Effectiveness) AND (Evidence OR Validation OR Empirical Support OR Empirical OR Support) AND (Missed OR Opportunities OR "Missed Opportunities" OR "Unapplied Patterns" OR Unapplied) AND (Formalization OR Standardization) AND (Adoption OR Time OR "Adoption Over Time" OR Trends OR Evolution) AND (Influence OR Impact OR "Cited Papers" OR Cited OR Papers) AND (Languages OR Transformation OR "Transformation Languages" OR DSL)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>['model transformation']</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>['advantages of patterns', 'benefits of patterns', 'case study', 'changes in pattern use', 'design pattern', 'empirical study', 'empirical validation', 'evidence of benefits', 'evolution of patterns', 'explicitly used', 'impact of pattern catalogs', 'implicitly used', 'in practice', 'industrial experience', 'influence of pattern literature', 'lack of pattern use', 'language support for patterns', 'missing patterns', 'model transformation', 'model-driven transformation', 'mt', 'mt language comparison', 'pattern adoption trends', 'pattern application', 'pattern classification', 'pattern expressiveness', 'pattern implementation', 'pattern taxonomy', 'pattern usage', 'patterns not applied', 'patterns not formalized', 'real-world', 'recognized pattern', 'should have used patterns', 'unformalized patterns', 'unrecognized pattern', 'use of pattern books']</t>
-        </is>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.02702702702702703</v>
-      </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>(model transformation OR MT OR "model-driven transformation" OR model OR transformation OR "driven transformation") AND ("design pattern" OR "pattern application" OR "pattern usage" OR "pattern implementation" OR design OR pattern OR application OR usage OR implementation) AND ("in practice" OR "real-world" OR "empirical study" OR "case study" OR "industrial experience" OR practice OR real OR world OR empirical OR study OR case OR industrial OR experience) AND ("pattern classification" OR "pattern taxonomy" OR classification OR taxonomy) AND ("explicitly used" OR "implicitly used" OR "recognized pattern" OR "unrecognized pattern" OR explicitly OR implicitly OR recognized OR unrecognized OR used) AND ("benefits of patterns" OR "advantages of patterns" OR "evidence of benefits" OR "empirical validation" OR benefits OR advantages OR evidence OR empirical OR validation OR patterns) AND ("patterns not applied" OR "should have used patterns" OR "lack of pattern use" OR applied OR lack) AND ("missing patterns" OR "unformalized patterns" OR "patterns not formalized" OR missing OR unformalized OR formalized) AND ("pattern adoption trends" OR "changes in pattern use" OR "evolution of patterns" OR adoption OR trends OR changes OR evolution) AND ("impact of pattern catalogs" OR "influence of pattern literature" OR "use of pattern books" OR impact OR influence OR literature OR catalogs OR books) AND ("MT language comparison" OR "pattern expressiveness" OR "language support for patterns" OR language OR comparison OR expressiveness OR support)</t>
-        </is>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>['adoption', 'adoption over time', 'advantages', 'architectural patterns', 'benefits', 'categories', 'cited papers', 'design patterns', 'dsl', 'effectiveness', 'empirical', 'empirical support', 'evidence', 'evolution', 'explicit', 'formalization', 'impact', 'implicit', 'influence', 'languages', 'mda', 'missed opportunities', 'model driven architecture', 'model transformation', 'model-driven transformation', 'mt', 'pattern classification', 'positive outcomes', 'practice', 'real-world', 'recognized', 'software patterns', 'standardization', 'transformation languages', 'trends', 'types', 'unapplied patterns', 'validation']</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>0.02631578947368421</v>
       </c>
       <c r="T4" t="n">
-        <v>0.01204819277108434</v>
+        <v>0.01694915254237288</v>
       </c>
     </row>
     <row r="5">
@@ -806,30 +806,30 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>("blockchain governance" OR "blockchain" OR "distributed ledger technology") AND ("governance" OR "management" OR "regulation" OR "control") AND ("building blocks" OR "components" OR "elements")</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
+          <t>("blockchain governance" OR "distributed ledger governance" OR "decentralized governance" OR "blockchain regulation" OR "governance" OR "governing" OR "management") AND ("building blocks" OR "components" OR "elements" OR "infrastructure" OR "foundations" OR "architecture")</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>(blockchain OR "blockchain governance" OR "distributed ledger" OR "distributed ledger governance" OR "decentralized" OR "decentralized governance" OR "blockchain regulation" OR "governance" OR "governing" OR "management" OR "govern" OR "regulate" OR "regulation") AND ("building blocks" OR "components" OR "elements" OR "infrastructure" OR "foundations" OR "architecture" OR "building" OR "block" OR "component" OR "element" OR "infrastructural" OR "foundation" OR "architectural")</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>['autonomous organization"and governance', 'blockchain ordistributed', 'decentralizedand ledger', 'ecosystem', 'management', 'platform']</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>['blockchain', 'blockchain governance', 'building blocks', 'components', 'control', 'distributed ledger technology', 'elements', 'governance', 'management', 'regulation']</t>
-        </is>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.06666666666666667</v>
-      </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>(blockchain OR "distributed ledger technology" OR "distributed ledger" OR "DLT" OR "block chain") AND (governance OR management OR regulation OR control OR "corporate governance" OR "IT governance" OR "risk management" OR "compliance") AND ("building blocks" OR components OR elements OR "core components" OR "fundamental elements" OR "basic building blocks")</t>
-        </is>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>['architecture', 'blockchain governance', 'blockchain regulation', 'building blocks', 'components', 'decentralized governance', 'distributed ledger governance', 'elements', 'foundations', 'governance', 'governing', 'infrastructure', 'management']</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>0.05555555555555555</v>
       </c>
       <c r="T5" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.03225806451612903</v>
       </c>
     </row>
     <row r="6">
@@ -878,27 +878,27 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>("model-based code reuse" OR "model driven code reuse" OR "model based software reuse" OR "model driven software reuse" OR "MCR") AND ("foundational knowledge" OR "body of knowledge" OR "underlying principles" OR "theoretical basis") AND ("approach" OR "method" OR "technique" OR "strategy") AND ("evaluation" OR "assessment" OR "validation" OR "testing") AND ("conclusion" OR "result" OR "finding" OR "outcome")</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
+          <t>("model checking" OR "model-checking" OR "modelchecker" OR "formal verification") AND (result OR results OR outcome OR outcomes OR analysis OR interpretation) AND ("foundational knowledge" OR "body of knowledge" OR "fundamental principles" OR "theoretical basis") AND (approach OR approaches OR method OR methods OR technique OR techniques OR strategy OR strategies OR development OR "tool support" OR "automated support") AND (evaluation OR evaluations OR assessment OR assessments OR validation OR validation OR verification OR verifications OR "empirical study" OR "case study" OR experiment OR experiments OR conclusion OR conclusions)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>(model OR models OR checking OR checkers OR "model checking" OR "model-checking" OR modelchecker OR "formal verification" OR "formal methods") AND (result OR results OR outcome OR outcomes OR analysis OR interpretation OR findings) AND (foundational OR foundation OR knowledge OR "foundational knowledge" OR "body of knowledge" OR fundamental OR principles OR "fundamental principles" OR theoretical OR basis OR "theoretical basis" OR theory) AND (approach OR approaches OR method OR methods OR technique OR techniques OR strategy OR strategies OR development OR develop OR "tool support" OR tool OR support OR "automated support" OR automation) AND (evaluation OR evaluations OR assessment OR assessments OR validation OR valid OR verification OR verifications OR "empirical study" OR empirical OR study OR "case study" OR case OR experiment OR experiments OR conclusion OR conclusions)</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>['code inspection', 'code review', 'formal inspection', 'software inspection']</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>['approach', 'assessment', 'body of knowledge', 'conclusion', 'evaluation', 'finding', 'foundational knowledge', 'mcr', 'method', 'model based software reuse', 'model driven code reuse', 'model driven software reuse', 'model-based code reuse', 'outcome', 'result', 'strategy', 'technique', 'testing', 'theoretical basis', 'underlying principles', 'validation']</t>
-        </is>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>(model AND based AND code AND reuse OR "model-based code reuse" OR model AND driven AND code AND reuse OR "model driven code reuse" OR model AND based AND software AND reuse OR "model based software reuse" OR model AND driven AND software AND reuse OR "model driven software reuse" OR MCR) AND (foundational AND knowledge OR body AND knowledge OR underlying AND principles OR theoretical AND basis OR "foundational knowledge" OR "body of knowledge" OR "underlying principles" OR "theoretical basis") AND (approach OR method OR technique OR strategy) AND (evaluation OR assessment OR validation OR testing) AND (conclusion OR result OR finding OR outcome)</t>
-        </is>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>['analysis', 'approach', 'approaches', 'assessment', 'assessments', 'automated support', 'body of knowledge', 'case study', 'conclusion', 'conclusions', 'development', 'empirical study', 'evaluation', 'evaluations', 'experiment', 'experiments', 'formal verification', 'foundational knowledge', 'fundamental principles', 'interpretation', 'method', 'methods', 'model checking', 'model-checking', 'modelchecker', 'outcome', 'outcomes', 'result', 'results', 'strategies', 'strategy', 'technique', 'techniques', 'theoretical basis', 'tool support', 'validation', 'validation', 'verification', 'verifications']</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -950,27 +950,27 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>("visual notation" OR "diagrammatic representation" OR "modeling language" OR UML OR BPMN OR ERD) AND ("Physics of Notations" OR "PoN theory") AND (analysis OR evaluation OR assessment OR validation) AND ("user requirements" OR usability OR "user experience" OR "cognitive aspects") AND (verifiability OR validation OR reliability OR accuracy)</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
+          <t>("visual notation" OR "visual notations" OR diagram OR diagrams OR model OR models OR "graphical representation" OR "graphical representations") AND (analysis OR analyses OR analyzed OR "notation analysis") AND ("Principles of Notation" OR "PoN theory" OR "PoN framework") AND (user OR users OR "user requirements" OR "user-centered" OR "user-centric") AND (verifiable OR verification OR "empirical analysis") AND (requirement OR requirements OR "requirements engineering")</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>((visual OR notation OR "visual notation" OR "visual notations" OR diagram OR diagrams OR model OR models OR graphical OR representation OR "graphical representation" OR "graphical representations") AND (analysis OR analyses OR analyzed OR notation OR "notation analysis") AND (principles OR notation OR "Principles of Notation" OR "PoN theory" OR "PoN framework") AND (user OR users OR requirements OR "user requirements" OR "user-centered" OR "user-centric") AND (verifiable OR verification OR empirical OR "empirical analysis") AND (requirement OR requirements OR engineering OR "requirements engineering"))</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>['“cognitive effectiveness”', '“diagram”', '“language”', '“modeling”', '“notation”', '“physics of notations”', '“visual”']</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>['accuracy', 'analysis', 'assessment', 'bpmn', 'cognitive aspects', 'diagrammatic representation', 'erd', 'evaluation', 'modeling language', 'physics of notations', 'pon theory', 'reliability', 'uml', 'usability', 'user experience', 'user requirements', 'validation', 'validation', 'verifiability', 'visual notation']</t>
-        </is>
-      </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>(visual OR visuals OR notation OR notations OR diagram OR diagrams OR diagrammatic OR representation OR representations OR model OR models OR modeling OR language OR languages OR UML OR BPMN OR ERD) AND (Physics OR Physics of Notations OR Physics of Notation OR PoN OR theory OR theories OR "PoN theory") AND (analysis OR analyses OR evaluation OR evaluations OR assessment OR assessments OR validate OR validates OR validation OR validations) AND (user OR users OR requirement OR requirements OR usability OR usabilities OR experience OR experiences OR "user requirements" OR "user experience" OR cognitive OR cognitives OR aspect OR aspects) AND (verifiability OR verifiable OR validation OR validations OR reliability OR reliable OR accuracy OR accurate)</t>
-        </is>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>['analyses', 'analysis', 'analyzed', 'diagram', 'diagrams', 'empirical analysis', 'graphical representation', 'graphical representations', 'model', 'models', 'notation analysis', 'pon framework', 'pon theory', 'principles of notation', 'requirement', 'requirements', 'requirements engineering', 'user', 'user requirements', 'user-centered', 'user-centric', 'users', 'verifiable', 'verification', 'visual notation', 'visual notations']</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1022,30 +1022,30 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>("semi-automatic configuration" OR "semi automatic configuration") AND ("product lines" OR "product line" OR "PL") AND (evaluation OR assessment OR validation) AND ("open challenges" OR "future research" OR limitations)</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
+          <t>("semi-automatic" OR "assisted" OR "automated") AND (configuration OR "set-up" OR arrangement OR parameterization) AND ("product line" OR "product family" OR "software product line" OR SPL OR variability OR customization OR extension) AND (evaluation OR assessment OR validation OR experiment OR "case study" OR performance) AND (challenge OR issue OR limitation OR gap OR "future work" OR "research direction")</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>("semi-automatic" OR "assisted" OR "automated" OR "automation" OR "automatic") AND (configuration OR "set-up" OR arrangement OR parameterization OR configure OR setup OR arrange OR parameterize) AND ("product line" OR "product family" OR "software product line" OR SPL OR variability OR customization OR extension OR "product lines" OR "product families" OR "software product lines" OR variant OR variants OR customizable OR extend) AND (evaluation OR assessment OR validation OR experiment OR "case study" OR performance OR evaluate OR assess OR validate OR experiment OR perform) AND (challenge OR issue OR limitation OR gap OR "future work" OR "research direction" OR challenges OR issues OR limitations OR gaps OR "future works" OR "research directions")</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>['attribute', 'confugyration', 'feature selection', 'non-functional', 'preference', 'product family', 'product line', 'product selection', 'quality', 'requirement', 'system family']</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>['assessment', 'evaluation', 'future research', 'limitations', 'open challenges', 'pl', 'product line', 'product lines', 'semi automatic configuration', 'semi-automatic configuration', 'validation']</t>
-        </is>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.04761904761904762</v>
-      </c>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>(("semi-automatic configuration" OR "semi automatic configuration" OR "semi-automatic" OR "semi automatic" OR "configuration")) AND (("product lines" OR "product line" OR "PL" OR "products" OR "lines")) AND ((evaluation OR assessment OR validation OR evaluate OR assess OR validate)) AND (("open challenges" OR "future research" OR limitations OR "open challenge" OR "future" OR "research" OR challenge))</t>
-        </is>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>['arrangement', 'assessment', 'assisted', 'automated', 'case study', 'challenge', 'configuration', 'customization', 'evaluation', 'experiment', 'extension', 'future work', 'gap', 'issue', 'limitation', 'parameterization', 'performance', 'product family', 'product line', 'research direction', 'semi-automatic', 'set-up', 'software product line', 'spl', 'validation', 'variability']</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>0.05714285714285714</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0303030303030303</v>
+        <v>0.03448275862068965</v>
       </c>
     </row>
     <row r="9">
@@ -1131,27 +1131,27 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>("software engineering" OR "software development" OR "software maintenance" OR "software testing" OR "requirements engineering" OR "software" OR "engineering") AND ("deep learning" OR "neural networks" OR "machine learning" OR CNN OR RNN OR transformer) AND ("software data" OR "code data" OR "data extraction" OR "data preprocessing" OR "feature engineering") AND ("baseline methods" OR benchmarks OR "reproducibility studies" OR "generalization performance")</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
+          <t>("deep learning" OR "DL" OR "neural network*" OR "machine learning") AND ("software engineering" OR "SE" OR "software development" OR "software design" OR "system engineering") AND (task OR tasks OR artifact OR artifacts OR data OR datum) AND (extract* OR pre-process* OR preprocess* OR analy* OR design OR evaluat*) AND (reproduc* OR generaliz*)</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>(deep learning OR DL OR neural network* OR machine learning OR deep OR learning OR network) AND (software engineering OR SE OR software development OR software design OR system engineering OR software OR engineering OR development OR design OR system) AND (task OR tasks OR artifact OR artifacts OR data OR datum) AND (extract* OR pre-process* OR preprocess* OR analy* OR design OR evaluat* OR extract OR process OR analy OR evaluate) AND (reproduc* OR generaliz* OR reproduc OR generalize)</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>['“deep”', '“learning”', '“neural”']</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>['baseline methods', 'benchmarks', 'cnn', 'code data', 'data extraction', 'data preprocessing', 'deep learning', 'engineering', 'feature engineering', 'generalization performance', 'machine learning', 'neural networks', 'reproducibility studies', 'requirements engineering', 'rnn', 'software', 'software data', 'software development', 'software engineering', 'software maintenance', 'software testing', 'transformer']</t>
-        </is>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>(software OR engineering OR "software engineering" OR "software development" OR development OR "software maintenance" OR maintenance OR "software testing" OR testing OR "requirements engineering" OR requirements OR "software" OR "engineering") AND (deep OR learning OR "deep learning" OR "neural networks" OR neural OR networks OR "machine learning" OR machine OR learning OR CNN OR RNN OR transformer) AND (software OR data OR "software data" OR "code data" OR code OR data OR "data extraction" OR extraction OR "data preprocessing" OR preprocessing OR "feature engineering" OR feature OR engineering) AND (baseline OR methods OR "baseline methods" OR benchmarks OR "reproducibility studies" OR reproducibility OR studies OR "generalization performance" OR generalization OR performance)</t>
-        </is>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>['analy*', 'artifact', 'artifacts', 'data', 'datum', 'deep learning', 'design', 'dl', 'evaluat*', 'extract*', 'generaliz*', 'machine learning', 'neural network*', 'pre-process*', 'preprocess*', 'reproduc*', 'se', 'software design', 'software development', 'software engineering', 'system engineering', 'task', 'tasks']</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1207,26 +1207,30 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>("software trust" OR "SECO trust" OR "software security trust") AND (definition OR concept OR factors OR criteria) AND ("software product selection" OR "software package manager selection" OR "software producing organization selection" OR "software engineer selection" OR "software selection") AND ("end-user" OR "organization" OR "company")</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
+          <t>("software trust" OR "SECO trust" OR "trust factors" OR "end-user organizations" OR "software products" OR "software package managers" OR "software producing organizations" OR "software engineers") AND ("defined" OR "selecting" OR "consider")</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>("software" OR "trust" OR "SECO" OR "factors" OR "end-user" OR "organizations" OR "products" OR "package" OR "managers" OR "producing" OR "engineers") AND ("defined" OR "selecting" OR "consider") OR ("software trust" OR "SECO trust" OR "trust factors" OR "end-user organizations" OR "software products" OR "software package managers" OR "software producing organizations" OR "software engineers") AND ("defined" OR "selecting" OR "consider")</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>['compoonent', 'credibility', 'dependency', 'developer', 'management', 'package', 'procenance', 'reputation', 'software', 'software ecosystem', 'trust', 'uncertainty']</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>['company', 'concept', 'criteria', 'definition', 'end-user', 'factors', 'organization', 'seco trust', 'software engineer selection', 'software package manager selection', 'software producing organization selection', 'software product selection', 'software security trust', 'software selection', 'software trust']</t>
-        </is>
-      </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>['consider', 'defined', 'end-user organizations', 'seco trust', 'selecting', 'software engineers', 'software package managers', 'software producing organizations', 'software products', 'software trust', 'trust factors']</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>0.09677419354838709</v>
       </c>
     </row>
     <row r="11">
@@ -1273,24 +1277,32 @@
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>("data mining" OR "sentiment analysis" OR "topic modeling" OR "classification" OR "machine learning") AND ("software distribution platforms" OR "app store reviews" OR "app reviews" OR "application reviews") AND ("domain dependency" OR "cross-domain" OR "transfer learning") AND ("review usefulness" OR "review quality" OR "helpful reviews") AND ("spam reviews" OR "fake reviews" OR "deceptive reviews") AND ("legitimate reviews" OR "genuine reviews" OR "authentic reviews") AND ("feature extraction" OR "feature identification" OR "feature mining") AND ("software features" OR "application features" OR "app features")</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>("data" OR "mining" OR "data mining" OR "sentiment" OR "analysis" OR "sentiment analysis" OR "topic" OR "modeling" OR "topic modeling" OR "classification" OR "machine" OR "learning" OR "machine learning") AND ("software" OR "distribution" OR "platforms" OR "software distribution platforms" OR "app" OR "store" OR "reviews" OR "app store reviews" OR "app reviews" OR "application" OR "reviews" OR "application reviews") AND ("domain" OR "dependency" OR "domain dependency" OR "cross-domain" OR "transfer" OR "learning" OR "transfer learning") AND ("review" OR "usefulness" OR "review usefulness" OR "review quality" OR "helpful" OR "reviews" OR "helpful reviews") AND ("spam" OR "reviews" OR "spam reviews" OR "fake" OR "reviews" OR "fake reviews" OR "deceptive" OR "reviews" OR "deceptive reviews") AND ("legitimate" OR "reviews" OR "legitimate reviews" OR "genuine" OR "reviews" OR "genuine reviews" OR "authentic" OR "reviews" OR "authentic reviews") AND ("feature" OR "extraction" OR "feature extraction" OR "identification" OR "feature identification" OR "feature mining") AND ("software" OR "features" OR "software features" OR "application" OR "features" OR "application features" OR "app" OR "features" OR "app features")</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>['analysis', 'app', 'application', 'apps', 'appstore', 'bug', 'comment', 'complain', 'data', 'ecosystem', 'expectation', 'feature', 'helpfulness', 'issue', 'market', 'mining', 'mobile', 'online', 'opinion', 'processing', 'quality', 'rating', 'request', 'requirement', 'review', 'sentiment', 'software', 'store', 'text', 'usefulness', 'user', 'vocabulary']</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>['app features', 'app reviews', 'app store reviews', 'application features', 'application reviews', 'authentic reviews', 'classification', 'cross-domain', 'data mining', 'deceptive reviews', 'domain dependency', 'fake reviews', 'feature extraction', 'feature identification', 'feature mining', 'genuine reviews', 'helpful reviews', 'legitimate reviews', 'machine learning', 'review quality', 'review usefulness', 'sentiment analysis', 'software distribution platforms', 'software features', 'spam reviews', 'topic modeling', 'transfer learning']</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>0.1392405063291139</v>
       </c>
     </row>
     <row r="12">
@@ -1339,24 +1351,32 @@
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>("visualization techniques" OR "visual representation" OR "visual modeling" OR "UML diagrams" OR "architectural views") AND ("software architecture" OR "system architecture" OR "software design" OR "application architecture") AND ("architecting activities" OR "software development" OR "system design" OR "architecture design")</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>(visualization OR techniques OR "visualization techniques" OR visual OR representation OR "visual representation" OR visual OR modeling OR "visual modeling" OR UML OR diagrams OR "UML diagrams" OR architectural OR views OR "architectural views") AND (software OR architecture OR "software architecture" OR system OR architecture OR "system architecture" OR software OR design OR "software design" OR application OR architecture OR "application architecture") AND (architecting OR activities OR "architecting activities" OR software OR development OR "software development" OR system OR design OR "system design" OR architecture OR design OR "architecture design")</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>['architecting', 'architectural', 'architecture', 'diagram', 'graphic', 'graphical', 'picture', 'structure', 'visual', 'visualization', 'visualize', 'visualizing']</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>['application architecture', 'architecting activities', 'architectural views', 'architecture design', 'software architecture', 'software design', 'software development', 'system architecture', 'system design', 'uml diagrams', 'visual modeling', 'visual representation', 'visualization techniques']</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>0.1351351351351351</v>
       </c>
     </row>
     <row r="13">
@@ -1409,22 +1429,30 @@
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>("UML" OR "Unified Modeling Language") AND ("method" OR "language" OR "technique" OR "approach") AND ("formal" OR "non-formal") AND ("diagram" OR "model") AND ("consistency" OR "inconsistency") AND ("problem" OR "issue" OR "error") AND ("extend" OR "support" OR "new") AND ("check" OR "validation")</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>(("UML" OR "Unified Modeling Language") OR "Unified" OR "Modeling Language" OR "Modeling") AND (("method" OR "language" OR "technique" OR "approach") OR "methodology" OR "formalism") AND (("formal" OR "non-formal") OR "semi-formal" OR "informal" OR "rigorous") AND (("diagram" OR "model") OR "modeling" OR "notation" OR "representation") AND (("consistency" OR "inconsistency") OR "validation" OR "correctness" OR "agreement") AND (("problem" OR "issue" OR "error") OR "defect" OR "fault" OR "bug" OR "challenge") AND (("extend" OR "support" OR "new") OR "enhance" OR "improve" OR "novel" OR "integration") AND (("check" OR "validation") OR "verification" OR "testing" OR "analysis")</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>['“consistency”', '“consistency”or “model”', '“inconsistency”', '“inconsistency”', '“management”', '“model”']</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>['approach', 'check', 'consistency', 'diagram', 'error', 'extend', 'formal', 'inconsistency', 'issue', 'language', 'method', 'model', 'new', 'non-formal', 'problem', 'support', 'technique', 'uml', 'unified modeling language', 'validation']</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
       <c r="T13" t="n">
         <v>0</v>
       </c>
@@ -1486,24 +1514,32 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>("search-based software testing" OR SBST OR "search based software engineering" OR SBSE) AND ("mutation testing" OR "mutation analysis" OR "fault injection") AND ("meta-heuristics" OR "genetic algorithms" OR "evolutionary algorithms" OR "particle swarm optimization" OR "simulated annealing") AND ("fitness function*" OR "objective function*") AND ("programming language*" OR "software language*")</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>(search OR "search-based" OR "search based" OR testing OR "software testing" OR SBST OR engineering OR "software engineering" OR SBSE) AND (mutation OR testing OR "mutation testing" OR analysis OR "mutation analysis" OR "fault injection") AND (metaheuristics OR "meta-heuristics" OR genetic OR algorithms OR "genetic algorithms" OR evolutionary OR "evolutionary algorithms" OR particle OR swarm OR optimization OR "particle swarm optimization" OR simulated OR annealing OR "simulated annealing") AND (fitness OR function* OR "fitness function*" OR objective OR "objective function*") AND (programming OR language* OR "programming language*" OR software OR "software language*")</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>['ant colony', 'evelutionary', 'genetic algorithms', 'genetic programming', 'heuristic', 'hill-climbing', 'meta-heuristic', 'metaheuristic', 'mutation analysis', 'mutation based test', 'mutation test', 'mutation testing', 'mutation-based test', 'oprimization', 'program mutation', 'search based', 'search-based', 'simulated annealing', 'tabu search']</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>['evolutionary algorithms', 'fault injection', 'fitness function*', 'genetic algorithms', 'meta-heuristics', 'mutation analysis', 'mutation testing', 'objective function*', 'particle swarm optimization', 'programming language*', 'sbse', 'sbst', 'search based software engineering', 'search-based software testing', 'simulated annealing', 'software language*']</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
+        <v>0.1290322580645161</v>
+      </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>0.1176470588235294</v>
       </c>
     </row>
     <row r="15">
@@ -1557,24 +1593,32 @@
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>(("code smell" OR "code smells" OR "code quality" OR "technical debt" OR "long method" OR "duplicate code") AND (effect OR impact OR influence OR consequence) AND ("experimental settings" OR "study design" OR methodology OR evaluation)) AND (findings convergence OR agreement OR consistency OR replication)</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>((("code smell" OR "code smells" OR "code" OR "smell" OR "code quality" OR "quality" OR "technical debt" OR "technical" OR "debt" OR "long method" OR "long" OR "method" OR "duplicate code" OR "duplicate") OR ("software defect" OR "software defects" OR "software" OR "defect")) AND (effect OR impact OR influence OR consequence) AND ("experimental settings" OR "experimental" OR "settings" OR "study design" OR "study" OR "design" OR methodology OR evaluation)) AND ("findings convergence" OR "findings" OR "convergence" OR agreement OR consistency OR replication)</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>['anti-patternandexperiment', 'controlled', 'disharmony', 'empirical', 'ethnography', 'smell', 'study', 'survey', '“action research”', '“code anomaly”', '“design anomaly”', '“design flaw”', '“exploratory analysis”']</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>['agreement', 'code quality', 'code smell', 'code smells', 'consequence', 'consistency', 'duplicate code', 'effect', 'evaluation', 'experimental settings', 'findings convergence', 'impact', 'influence', 'long method', 'methodology', 'replication', 'study design', 'technical debt']</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>0.0425531914893617</v>
       </c>
     </row>
     <row r="16">
@@ -1622,22 +1666,30 @@
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>("Social Interaction Agent*" OR "SIA") AND (Input* OR Process* OR Output* OR Usability OR "User Experience" OR "Human Factors")</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>(Social Interaction Agent* OR SIA OR "Social" OR "Interaction" OR "Agent") AND (Input* OR Process* OR Output* OR Usability OR "User Experience" OR "Human Factors" OR "User" OR "Experience" OR "Human" OR "Factor")</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>['existing systems', 'legacy', 'migration', 'modernization', 'object-oriented', 're-engineering', 'service identification', 'service mining', 'service packaging', 'transformation']</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>['human factors', 'input*', 'output*', 'process*', 'sia', 'social interaction agent*', 'usability', 'user experience']</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
       <c r="T16" t="n">
         <v>0</v>
       </c>
@@ -1707,24 +1759,32 @@
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>("agile methods" OR "agile development" OR scrum OR lean) AND ("method tailoring" OR "method adaptation" OR "process tailoring" OR "situational method engineering") AND ("methodological aspects" OR "research methods" OR methodology OR "research design") AND (practicality OR "empirical studies" OR "case studies" OR "real-world application") AND ("tailoring criteria" OR "selection criteria" OR factors OR guidelines)</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>(agile OR "agile methods" OR "agile development" OR scrum OR lean) AND (tailoring OR "method tailoring" OR "method adaptation" OR "process tailoring" OR "situational method engineering" OR "situational method" OR "method engineering") AND ("methodological aspects" OR "research methods" OR methodology OR method OR research OR "research design") AND (practicality OR practical OR "empirical studies" OR "case studies" OR "real-world application" OR "real world" OR application) AND (criteria OR "tailoring criteria" OR "selection criteria" OR factors OR guidelines OR guideline OR selecting OR selecting)</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>['adoption orfdd', 'adoption orkanban', 'adoption orlean', 'adoption orscrum', 'adoption orxp', 'adoption or“feature driven development”', 'agile', 'method', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'practice', 'select', 'select oragile', 'select orfdd', 'select orkanban', 'select orlean', 'select orxp', 'select or“feature driven development”', 'tailoring orfdd', 'tailoring orkanban', 'tailoring orlean', 'tailoring orscrum', 'tailoring orscrum', 'tailoring orxp', 'tailoring or“feature driven development”']</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>['agile development', 'agile methods', 'case studies', 'empirical studies', 'factors', 'guidelines', 'lean', 'method adaptation', 'method tailoring', 'methodological aspects', 'methodology', 'practicality', 'process tailoring', 'real-world application', 'research design', 'research methods', 'scrum', 'selection criteria', 'situational method engineering', 'tailoring criteria']</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="18">
@@ -1772,22 +1832,30 @@
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr">
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>("agile practice*" OR "agile method*" OR "scrum" OR "kanban" OR "extreme programming") AND ("critical success factor*" OR CSF OR ("success factor*" AND "software development")) AND ("global software development" OR GSD OR "distributed software development" OR "offshore software development") AND (vendor* OR "software compan*" OR "software provider*") AND ("green software" OR "sustainable software" OR "environmentally friendly software" OR ("software development" AND (sustainability OR "green IT" OR "environmental impact"))</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>(agile OR practice* OR agile practice* OR method* OR agile method* OR scrum OR kanban OR "extreme programming" OR XP) AND (critical OR success OR factor* OR critical success factor* OR CSF OR ("success factor*" AND "software development")) AND (global OR software OR development OR "global software development" OR GSD OR distributed OR "distributed software development" OR offshore OR "offshore software development") AND (vendor* OR software OR compan* OR "software compan*" OR provider* OR "software provider*") AND (green OR sustainable OR environmentally OR software OR "green software" OR "sustainable software" OR "environmentally friendly software" OR ("software development" AND (sustainability OR "green IT" OR "environmental impact" OR green OR IT OR impact)))</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
         <is>
           <t>['“agile methods”', '“agile”', '“green agile”', '“green software engineering”', '“green software”', '“greener software”', '“practices”', '“solutions”', '“sustainable software”']</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>['agile method*', 'agile practice*', 'critical success factor*', 'csf', 'distributed software development', 'environmental impact', 'environmentally friendly software', 'extreme programming', 'global software development', 'green it', 'green software', 'gsd', 'kanban', 'offshore software development', 'scrum', 'software compan*', 'software development', 'software development', 'software provider*', 'success factor*', 'sustainability', 'sustainable software', 'vendor*']</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
       <c r="T18" t="n">
         <v>0</v>
       </c>
@@ -1840,24 +1908,32 @@
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr">
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>("CMMI-DEV" OR "Capability Maturity Model Integration for Development" OR "CMMI") AND (Agile OR Scrum OR Kanban OR "Extreme Programming" OR XP) AND (Web OR "Web Environment" OR "Web Development" OR "Web Application" OR "Web Technologies") AND (maturity OR "maturity level" OR "process improvement")</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>("CMMI-DEV" OR "Capability Maturity Model Integration for Development" OR "CMMI" OR "Capability Maturity Model" OR Capability OR Maturity OR Integration OR Development) AND (Agile OR Scrum OR Kanban OR "Extreme Programming" OR XP OR Agility) AND (Web OR "Web Environment" OR "Web Development" OR "Web Application" OR "Web Technologies" OR Website OR Websites OR "World Wide Web") AND (maturity OR "maturity level" OR "process improvement" OR process OR improvement OR improve OR maturing)</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
         <is>
           <t>['agile', 'agility', 'capability maturity model', 'cmmi', 'extreme programming', 'scrum', 'web', 'web engineering']</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>['agile', 'capability maturity model integration for development', 'cmmi', 'cmmi-dev', 'extreme programming', 'kanban', 'maturity', 'maturity level', 'process improvement', 'scrum', 'web', 'web application', 'web development', 'web environment', 'web technologies', 'xp']</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>0.2631578947368421</v>
+      </c>
       <c r="T19" t="n">
-        <v>0</v>
+        <v>0.2413793103448276</v>
       </c>
     </row>
     <row r="20">
@@ -1904,22 +1980,30 @@
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr">
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>((data collection methods OR survey OR study design) AND (curriculum models OR bodies of knowledge OR study design) AND (SE skills OR software engineering skills OR important SE subjects OR least important SE subjects) AND (knowledge gaps OR deficiencies in SE subjects OR topics with high deficiencies) AND (soft skills OR importance of soft skills OR balance of soft and hard skills) AND (data sample characteristics OR number of data points OR participants OR job advertisements OR survey coverage) AND (educational recommendations OR study recommendations OR educational guidelines) AND (meta-analysis findings OR comparison of findings OR previous review papers))</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>((data collection methods OR data collection OR collection methods OR survey OR study design OR study OR design) AND (curriculum models OR curriculum OR models OR bodies of knowledge OR bodies OR knowledge OR study design OR study OR design) AND (SE skills OR software engineering skills OR software OR engineering OR skills OR important SE subjects OR important OR SE OR subjects OR least important SE subjects OR least OR important OR SE OR subjects) AND (knowledge gaps OR knowledge OR gaps OR deficiencies in SE subjects OR deficiencies OR SE OR subjects OR topics with high deficiencies OR topics OR deficiencies) AND (soft skills OR soft OR skills OR importance of soft skills OR importance OR soft OR skills OR balance of soft and hard skills OR balance OR soft OR hard OR skills) AND (data sample characteristics OR data OR sample OR characteristics OR number of data points OR number OR data OR points OR participants OR job advertisements OR job OR advertisements OR survey coverage OR survey OR coverage) AND (educational recommendations OR educational OR recommendations OR study recommendations OR study OR recommendations OR educational guidelines OR educational OR guidelines) AND (meta-analysis findings OR meta-analysis OR findings OR comparison of findings OR comparison OR findings OR previous review papers OR previous OR review OR papers))</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>['desired skills', 'educational needs', 'essential competencies', 'knowledge needs', 'knowledge requirements', 'skill requirements', 'software developers', 'software engineers']</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>['balance of soft', 'bodies of knowledge', 'comparison of findings', 'curriculum models', 'data collection methods', 'data sample characteristics', 'deficiencies in se subjects', 'educational guidelines', 'educational recommendations', 'hard skills', 'importance of soft skills', 'important se subjects', 'job advertisements', 'knowledge gaps', 'least important se subjects', 'meta-analysis findings', 'number of data points', 'participants', 'previous review papers', 'se skills', 'soft skills', 'software engineering skills', 'study design', 'study design', 'study recommendations', 'survey', 'survey coverage', 'topics with high deficiencies']</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
       <c r="T20" t="n">
         <v>0</v>
       </c>
@@ -1972,22 +2056,30 @@
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr">
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>(app OR review OR analyses OR app-review OR review-analyses) AND (techniques) AND (software OR engineering OR activities OR software-engineering OR engineering-activities OR software design OR system engineering) AND (empirically OR evaluated) AND (support OR software OR engineers OR support-software OR software-engineers OR support-engineers)</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>(app OR review OR analyses OR app-review OR review-analyses OR app OR review OR analyses) AND (techniques OR technique OR technical OR tech) AND (software OR engineering OR activities OR software-engineering OR engineering-activities OR software design OR system engineering OR software OR engineering OR activities) AND (empirically OR evaluated OR empirical OR evaluation) AND (support OR software OR engineers OR support-software OR software-engineers OR support-engineers OR support OR software OR engineers)</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
         <is>
           <t>["'app review'", "'app store review'", "'app store'", "'requirement engineering'", "'software coding'", "'software configuration'", "'software construction'", "'software design'", "'software development'", "'software engineering'", "'software maintenance'", "'software quality'", "'software requirement'", "'software testing'", "'user feedback'", "'user review'"]</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>['activities', 'analyses', 'app', 'app-review', 'empirically', 'engineering', 'engineering-activities', 'engineers', 'evaluated', 'review', 'review-analyses', 'software', 'software', 'software design', 'software-engineering', 'software-engineers', 'support', 'support-engineers', 'support-software', 'system engineering', 'techniques']</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
       <c r="T21" t="n">
         <v>0</v>
       </c>
@@ -2037,22 +2129,30 @@
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr">
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>("offshore development" OR "offshore software development" OR "IT outsourcing") AND ("vendor" OR "service provider") AND ("reliability" OR "trustworthiness") AND ("challenges" OR "obstacles" OR "problems" OR "issues") AND ("impact" OR "effect") AND ("prioritization" OR "ranking") AND ("categorization" OR "classification")</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>(("offshore development" OR "offshore software development" OR "IT outsourcing" OR "offshore" OR "development" OR "software" OR "offshore software" OR "outsourcing")) AND (( "vendor" OR "service provider" OR "service" OR "provider" OR "vendors")) AND (("reliability" OR "trustworthiness" OR "trust")) AND (("challenges" OR "obstacles" OR "problems" OR "issues" OR "challenge" OR "obstacle" OR "problem")) AND (("impact" OR "effect" OR "impacts" OR "effects" OR "effected")) AND (("prioritization" OR "ranking" OR "categorization" OR "classification" OR "prioritize" OR "rank" OR "ranks" OR "category" OR "classify"))</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
         <is>
           <t>['dealer', 'developer', 'marketer', 'merchant', 'retailer', 'salesperson', 'seller', 'service-provider', 'trader', 'wholesaler”', '“barriers”', '“challenges”', '“critical factors”', '“global software development”', '“hurdles”', '“issues”', '“obstacles”', '“risk analysis”', '“risks”', '“software outsourcing development”', '“software outsourcing”', '“vendor']</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>['categorization', 'challenges', 'classification', 'effect', 'impact', 'issues', 'it outsourcing', 'obstacles', 'offshore development', 'offshore software development', 'prioritization', 'problems', 'ranking', 'reliability', 'service provider', 'trustworthiness', 'vendor']</t>
+        </is>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
       <c r="T22" t="n">
         <v>0</v>
       </c>
@@ -2101,24 +2201,32 @@
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>("conceptualized ontologies" OR ontology OR ontologies) AND ("software testing" OR software OR testing OR "software test") AND (domain OR concepts OR relationships OR properties OR axioms) AND (classification OR classified)</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>(conceptualized OR concept OR "conceptualized ontologies" OR ontology OR ontologies) AND ("software testing" OR software OR testing OR "software test" OR "software applications" OR application OR applies) AND (domain OR concepts OR relationships OR properties OR axioms OR characteristic OR feature OR attribute) AND (classification OR classified OR categorize OR "categorized")</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
         <is>
           <t>['ontologies', 'ontology', 'software test', 'software testing']</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>['axioms', 'classification', 'classified', 'concepts', 'conceptualized ontologies', 'domain', 'ontologies', 'ontology', 'properties', 'relationships', 'software', 'software test', 'software testing', 'testing']</t>
+        </is>
+      </c>
+      <c r="S23" t="n">
+        <v>0.2857142857142857</v>
+      </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="24">
@@ -2169,22 +2277,30 @@
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>("experience curve" OR "learning curve" OR "progress function" OR "cost reduction") AND ("software engineering" OR "software development" OR "software design" OR "software lifecycle" OR "SW engineering")</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>(experience OR curve OR "experience curve" OR learning OR "learning curve" OR progress OR function OR "progress function" OR cost OR reduction OR "cost reduction") AND (software OR engineering OR design OR development OR lifecycle OR "software engineering" OR "software development" OR "software design" OR "software lifecycle" OR "SW engineering" OR SW)</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>['“experience curve”', '“learning curve”', '“software development”', '“software engineering”', '“software process”', '“software project”']</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>['cost reduction', 'experience curve', 'learning curve', 'progress function', 'software design', 'software development', 'software engineering', 'software lifecycle', 'sw engineering']</t>
+        </is>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
       <c r="T24" t="n">
         <v>0</v>
       </c>
@@ -2234,22 +2350,30 @@
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr">
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>("IT personnel" OR "information technology staff" OR "computer staff" OR "IT employees" OR "technology workers") AND ("intentions to leave" OR "turnover intention" OR "employee turnover" OR "attrition" OR "job leaving") AND ("workplace" OR "organization" OR "company" OR "employment")</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>(("IT personnel" OR "information technology staff" OR "computer staff" OR "IT employees" OR "technology workers" OR "IT support" OR "computer technicians" OR "information systems staff") AND ("intentions to leave" OR "turnover intention" OR "employee turnover" OR "attrition" OR "job leaving" OR "employee retention" OR "retention" OR "quit" OR "resignation") AND ("workplace" OR "organization" OR "company" OR "employment" OR "organisation" OR "establishment" OR "place of work"))</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>['“employee retention”', '“employees retention”', '“intention for turnover”', '“intention to leave”', '“intention to quit”', '“intention to stay”', '“intention to withdraw”', '“is employee”', '“is manager”', '“is personnel”', '“is professional”', '“is workforce”', '“it employee”', '“it manager”', '“it personnel”', '“it professional”', '“it worker”', '“it workforce”', '“leave intention”', '“manager retention”', '“managers retention”', '“personnel retention”', '“professional retention”', '“professionals retention”and “is worker”', '“quit intention”', '“software designer”', '“software developer”', '“software engineer”', '“software manager”', '“software programmer”', '“software project manager”', '“stay intention”', '“system analyst”', '“turnover intention”', '“withdrawal intention”', '“worker retention”', '“workers retention”']</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>['attrition', 'company', 'computer staff', 'employee turnover', 'employment', 'information technology staff', 'intentions to leave', 'it employees', 'it personnel', 'job leaving', 'organization', 'technology workers', 'turnover intention', 'workplace']</t>
+        </is>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
       <c r="T25" t="n">
         <v>0</v>
       </c>
@@ -2307,24 +2431,32 @@
           <t>An essential requirement is the integration of user experience methods in Agile software development. Based on this, the development of positive user experience must be managed. We understand management in general as a combination of a goal, a strategy, and resources. When applied to UX, user experience management consists of a UX goal, a UX strategy, and UX resources.</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>("UX Management" OR "User Experience Management") AND (Agile OR Scrum OR Sprint) AND ("Software Development" OR "Software Engineering") AND ("User Experience" OR UX OR Usability OR "User Interface" OR "Interaction Design") AND (Planning OR Control OR Strategy OR Resources) AND (Retrospective OR Improvement OR Efficiency OR Effectiveness)</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>((UX OR "User Experience" OR Management) AND ("UX Management" OR "User Experience Management")) AND (Agile OR Scrum OR Sprint) AND ((Software OR Development OR Engineering) AND ("Software Development" OR "Software Engineering")) AND ((User OR Experience OR Usability OR "User Interface" OR Interaction OR Design) AND ("User Experience" OR UX OR Usability OR "User Interface" OR "Interaction Design")) AND ((Planning OR Control OR Strategy OR Resources) AND (Planning OR Control OR Strategy OR Resources)) AND ((Retrospective OR Improvement OR Efficiency OR Effectiveness) AND (Retrospective OR Improvement OR Efficiency OR Effectiveness))</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
         <is>
           <t>['agile', 'hcd', 'hci', 'hmi', 'kanban', 'lean', 'scrum', 'ucd', 'usability', 'ux', '“design thinking”and“user experience”', '“extreme programming”']</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>['nan']</t>
-        </is>
-      </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>['agile', 'control', 'effectiveness', 'efficiency', 'improvement', 'interaction design', 'planning', 'resources', 'retrospective', 'scrum', 'software development', 'software engineering', 'sprint', 'strategy', 'usability', 'user experience', 'user experience management', 'user interface', 'ux', 'ux management']</t>
+        </is>
+      </c>
+      <c r="S26" t="n">
+        <v>0.1428571428571428</v>
+      </c>
       <c r="T26" t="n">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>